<commit_message>
modified:   SECTOR_ETF/ETF_Result.xlsx 	renamed:    "SECTOR_ETF/sectorETF_Ret&Vol2-\354\227\254\352\270\260\353\266\200\355\204\260.py" -> SECTOR_ETF/sectorETF_Ret&Vol2.py 	new file:   "SECTOR_ETF/sectorETF_simple\354\241\260\355\225\2513-1.py" 	modified:   TQQQ_MA/TQQQ_Results.xlsx
</commit_message>
<xml_diff>
--- a/TQQQ_MA/TQQQ_Results.xlsx
+++ b/TQQQ_MA/TQQQ_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilpus\PythonProjects\git_folder\TQQQ_MA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC320883-5BC2-4772-8541-4B8D7579DFB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA228662-8D5B-409D-80AD-B10B33A4BA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Strategy" sheetId="2" r:id="rId1"/>
     <sheet name="BH" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -74,9 +74,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.0%"/>
-    <numFmt numFmtId="179" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="177" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,13 +106,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="맑은 고딕"/>
@@ -121,9 +115,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -177,25 +169,25 @@
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="백분율" xfId="1" builtinId="5"/>
@@ -502,10 +494,10 @@
   <dimension ref="A1:T52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="15.625" customWidth="1"/>
     <col min="3" max="3" width="9" style="1"/>
@@ -519,2321 +511,2325 @@
     <col min="16" max="16" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:20">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="12">
+    <row r="2" spans="1:20">
+      <c r="A2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="9">
         <v>20</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="10">
         <v>0.31350248283862597</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="10">
         <v>0.23451554825998611</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="10">
         <v>-0.291284356926651</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="11">
         <v>1.08183789597152</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="11">
         <v>0.9615870167171322</v>
       </c>
-      <c r="H2" s="12">
+      <c r="H2" s="9">
         <v>249</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="3">
+      <c r="I2" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="12">
         <v>20</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="13">
         <v>0.27790150218757531</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="13">
         <v>-0.42747568914174999</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2" s="14">
         <v>0.86189220862270188</v>
       </c>
-      <c r="N2" s="5">
+      <c r="N2" s="14">
         <v>0.93341196824536277</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="P2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="10">
+      <c r="Q2" s="7">
         <v>0.3457671090136043</v>
       </c>
-      <c r="R2" s="10">
+      <c r="R2" s="7">
         <v>-0.81659848664579748</v>
       </c>
-      <c r="S2" s="11">
+      <c r="S2" s="8">
         <v>0.79451975814654963</v>
       </c>
-      <c r="T2" s="11">
+      <c r="T2" s="8">
         <v>1.0186417049537391</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="9">
+    <row r="3" spans="1:20">
+      <c r="A3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="6">
         <v>235</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="7">
         <v>0.30296649530744801</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="7">
         <v>0.20526531622096281</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="7">
         <v>-0.50095002650463971</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="8">
         <v>0.9591952499744979</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="8">
         <v>0.84951856239170964</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="6">
         <v>74</v>
       </c>
-      <c r="I3" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="9">
+      <c r="I3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="6">
         <v>235</v>
       </c>
-      <c r="K3" s="10">
+      <c r="K3" s="7">
         <v>0.3407663344986851</v>
       </c>
-      <c r="L3" s="10">
+      <c r="L3" s="7">
         <v>-0.5009500265046396</v>
       </c>
-      <c r="M3" s="11">
+      <c r="M3" s="8">
         <v>0.89366034415812534</v>
       </c>
-      <c r="N3" s="11">
+      <c r="N3" s="8">
         <v>1.0068963592198861</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="3">
+      <c r="Q3" s="1">
+        <f>Q2*0.78</f>
+        <v>0.26969834503061135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="12">
         <v>225</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="13">
         <v>0.30190929481146078</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="13">
         <v>0.21167755928094631</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="13">
         <v>-0.5009500265046396</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="14">
         <v>0.96062949851820767</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="14">
         <v>0.84812514606548339</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="12">
         <v>78</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="3">
+      <c r="I4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="12">
         <v>225</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="13">
         <v>0.35553837649014097</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="13">
         <v>-0.50095002650463971</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="14">
         <v>0.92201759940024808</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="14">
         <v>1.039526449834302</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="9">
+    <row r="5" spans="1:20">
+      <c r="A5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="6">
         <v>240</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="7">
         <v>0.30164784523312638</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="7">
         <v>0.20504026914507831</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="7">
         <v>-0.5009500265046396</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="8">
         <v>0.95577326265075535</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="8">
         <v>0.84761365579705961</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="6">
         <v>74</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="9">
+      <c r="I5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="6">
         <v>240</v>
       </c>
-      <c r="K5" s="10">
+      <c r="K5" s="7">
         <v>0.32538275740023642</v>
       </c>
-      <c r="L5" s="10">
+      <c r="L5" s="7">
         <v>-0.50095002650463949</v>
       </c>
-      <c r="M5" s="11">
+      <c r="M5" s="8">
         <v>0.86555167141145284</v>
       </c>
-      <c r="N5" s="11">
+      <c r="N5" s="8">
         <v>0.97125448546796833</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="9">
+    <row r="6" spans="1:20">
+      <c r="A6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="6">
         <v>230</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="7">
         <v>0.30099064575000778</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="7">
         <v>0.2039386402356986</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="7">
         <v>-0.5009500265046396</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="8">
         <v>0.95567758387911106</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="8">
         <v>0.84459751853637588</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="6">
         <v>76</v>
       </c>
-      <c r="I6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="9">
+      <c r="I6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="6">
         <v>230</v>
       </c>
-      <c r="K6" s="10">
+      <c r="K6" s="7">
         <v>0.34357021112518499</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="7">
         <v>-0.5009500265046396</v>
       </c>
-      <c r="M6" s="11">
+      <c r="M6" s="8">
         <v>0.90015215640647117</v>
       </c>
-      <c r="N6" s="11">
+      <c r="N6" s="8">
         <v>1.016972700705232</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="9">
+    <row r="7" spans="1:20">
+      <c r="A7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="6">
         <v>245</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="7">
         <v>0.29259407593491388</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="7">
         <v>0.19592902025502301</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="7">
         <v>-0.54658409585796952</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="8">
         <v>0.9328052231372006</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="8">
         <v>0.82740223583628725</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="6">
         <v>80</v>
       </c>
-      <c r="I7" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="9">
+      <c r="I7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="6">
         <v>245</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7" s="7">
         <v>0.31512975712359398</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7" s="7">
         <v>-0.55066316741117627</v>
       </c>
-      <c r="M7" s="11">
+      <c r="M7" s="8">
         <v>0.84669551370874596</v>
       </c>
-      <c r="N7" s="11">
+      <c r="N7" s="8">
         <v>0.95095862005144982</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="9">
+    <row r="8" spans="1:20">
+      <c r="A8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="6">
         <v>250</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="7">
         <v>0.2877585913621763</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="7">
         <v>0.19553940842205941</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="7">
         <v>-0.60565845947431463</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="8">
         <v>0.91607230193569622</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="8">
         <v>0.81157262451384393</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="6">
         <v>78</v>
       </c>
-      <c r="I8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="9">
+      <c r="I8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="6">
         <v>250</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="7">
         <v>0.31079676524372929</v>
       </c>
-      <c r="L8" s="10">
+      <c r="L8" s="7">
         <v>-0.61060622705093026</v>
       </c>
-      <c r="M8" s="11">
+      <c r="M8" s="8">
         <v>0.83608286618844685</v>
       </c>
-      <c r="N8" s="11">
+      <c r="N8" s="8">
         <v>0.94024902198733107</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="9">
+    <row r="9" spans="1:20">
+      <c r="A9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="6">
         <v>255</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="7">
         <v>0.28451038959223102</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="7">
         <v>0.19551690209017011</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="7">
         <v>-0.6056584594743144</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="8">
         <v>0.90743426289835649</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="8">
         <v>0.80644593696387246</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="6">
         <v>84</v>
       </c>
-      <c r="I9" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" s="9">
+      <c r="I9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="6">
         <v>255</v>
       </c>
-      <c r="K9" s="10">
+      <c r="K9" s="7">
         <v>0.30301393938375282</v>
       </c>
-      <c r="L9" s="10">
+      <c r="L9" s="7">
         <v>-0.62842942300509563</v>
       </c>
-      <c r="M9" s="11">
+      <c r="M9" s="8">
         <v>0.82213940114650441</v>
       </c>
-      <c r="N9" s="11">
+      <c r="N9" s="8">
         <v>0.92606090040364586</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="9">
+    <row r="10" spans="1:20">
+      <c r="A10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="6">
         <v>220</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="7">
         <v>0.28357799383279558</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="7">
         <v>0.19413438987806869</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="7">
         <v>-0.50095002650463949</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="8">
         <v>0.91582757802337722</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="8">
         <v>0.80292435419619268</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="6">
         <v>84</v>
       </c>
-      <c r="I10" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J10" s="9">
+      <c r="I10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="6">
         <v>220</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="7">
         <v>0.3400360048190969</v>
       </c>
-      <c r="L10" s="10">
+      <c r="L10" s="7">
         <v>-0.5009500265046396</v>
       </c>
-      <c r="M10" s="11">
+      <c r="M10" s="8">
         <v>0.89443725903147553</v>
       </c>
-      <c r="N10" s="11">
+      <c r="N10" s="8">
         <v>1.00391586712041</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="9">
+    <row r="11" spans="1:20">
+      <c r="A11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="6">
         <v>30</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="7">
         <v>0.28225321520097341</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="7">
         <v>0.1772766664807337</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="7">
         <v>-0.51510799750694858</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="8">
         <v>0.97385564543941416</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="8">
         <v>0.8494650727634685</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="6">
         <v>198</v>
       </c>
-      <c r="I11" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J11" s="9">
+      <c r="I11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" s="6">
         <v>30</v>
       </c>
-      <c r="K11" s="10">
+      <c r="K11" s="7">
         <v>0.19536548633501871</v>
       </c>
-      <c r="L11" s="10">
+      <c r="L11" s="7">
         <v>-0.62585427405495953</v>
       </c>
-      <c r="M11" s="11">
+      <c r="M11" s="8">
         <v>0.67170930084762626</v>
       </c>
-      <c r="N11" s="11">
+      <c r="N11" s="8">
         <v>0.7098334823559268</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="9">
+    <row r="12" spans="1:20">
+      <c r="A12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="6">
         <v>25</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="7">
         <v>0.2738345283871515</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="7">
         <v>0.18410873017369481</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="7">
         <v>-0.38563817077993728</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="8">
         <v>0.95996295370058216</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="8">
         <v>0.82709313691467556</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="6">
         <v>212</v>
       </c>
-      <c r="I12" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J12" s="9">
+      <c r="I12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="6">
         <v>25</v>
       </c>
-      <c r="K12" s="10">
+      <c r="K12" s="7">
         <v>0.17396092778791331</v>
       </c>
-      <c r="L12" s="10">
+      <c r="L12" s="7">
         <v>-0.63670001783107799</v>
       </c>
-      <c r="M12" s="11">
+      <c r="M12" s="8">
         <v>0.62538526871140354</v>
       </c>
-      <c r="N12" s="11">
+      <c r="N12" s="8">
         <v>0.65584517561437572</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="9">
+    <row r="13" spans="1:20">
+      <c r="A13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6">
         <v>215</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="7">
         <v>0.27255874829210808</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="7">
         <v>0.18524796376012609</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="7">
         <v>-0.5009500265046396</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="8">
         <v>0.8886034787621131</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="8">
         <v>0.77517006494456953</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="6">
         <v>84</v>
       </c>
-      <c r="I13" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J13" s="9">
+      <c r="I13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J13" s="6">
         <v>215</v>
       </c>
-      <c r="K13" s="10">
+      <c r="K13" s="7">
         <v>0.32775698327168667</v>
       </c>
-      <c r="L13" s="10">
+      <c r="L13" s="7">
         <v>-0.50095002650463971</v>
       </c>
-      <c r="M13" s="11">
+      <c r="M13" s="8">
         <v>0.87259073011794919</v>
       </c>
-      <c r="N13" s="11">
+      <c r="N13" s="8">
         <v>0.97683539360092086</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="9">
+    <row r="14" spans="1:20">
+      <c r="A14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6">
         <v>195</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="7">
         <v>0.27092673052752159</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="7">
         <v>0.18801889643746561</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="7">
         <v>-0.50142636353316727</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="8">
         <v>0.88715653056065891</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="8">
         <v>0.77640400929337783</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="6">
         <v>84</v>
       </c>
-      <c r="I14" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J14" s="9">
+      <c r="I14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" s="6">
         <v>195</v>
       </c>
-      <c r="K14" s="10">
+      <c r="K14" s="7">
         <v>0.34146466620505511</v>
       </c>
-      <c r="L14" s="10">
+      <c r="L14" s="7">
         <v>-0.50142636353316716</v>
       </c>
-      <c r="M14" s="11">
+      <c r="M14" s="8">
         <v>0.90014868275122739</v>
       </c>
-      <c r="N14" s="11">
+      <c r="N14" s="8">
         <v>1.0104856876884949</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="9">
+    <row r="15" spans="1:20">
+      <c r="A15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="6">
         <v>210</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="7">
         <v>0.27057227432599928</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="7">
         <v>0.18435806128561461</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="7">
         <v>-0.5009500265046396</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="8">
         <v>0.88354321771042632</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="8">
         <v>0.77035571697844474</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="6">
         <v>83</v>
       </c>
-      <c r="I15" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J15" s="9">
+      <c r="I15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" s="6">
         <v>210</v>
       </c>
-      <c r="K15" s="10">
+      <c r="K15" s="7">
         <v>0.33993285625658909</v>
       </c>
-      <c r="L15" s="10">
+      <c r="L15" s="7">
         <v>-0.5009500265046396</v>
       </c>
-      <c r="M15" s="11">
+      <c r="M15" s="8">
         <v>0.89479820227442608</v>
       </c>
-      <c r="N15" s="11">
+      <c r="N15" s="8">
         <v>1.004861939491646</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="9">
+    <row r="16" spans="1:20">
+      <c r="A16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="6">
         <v>200</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="7">
         <v>0.26219864556704398</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="7">
         <v>0.18035718929032571</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="7">
         <v>-0.50142636353316727</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="8">
         <v>0.8638071542106005</v>
       </c>
-      <c r="G16" s="11">
+      <c r="G16" s="8">
         <v>0.75255916669628509</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="6">
         <v>87</v>
       </c>
-      <c r="I16" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J16" s="9">
+      <c r="I16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" s="6">
         <v>200</v>
       </c>
-      <c r="K16" s="10">
+      <c r="K16" s="7">
         <v>0.3335134877213155</v>
       </c>
-      <c r="L16" s="10">
+      <c r="L16" s="7">
         <v>-0.50142636353316727</v>
       </c>
-      <c r="M16" s="11">
+      <c r="M16" s="8">
         <v>0.88428987586534857</v>
       </c>
-      <c r="N16" s="11">
+      <c r="N16" s="8">
         <v>0.99069723402608934</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="9">
+    <row r="17" spans="1:14">
+      <c r="A17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="6">
         <v>15</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="7">
         <v>0.2543562048572825</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="7">
         <v>0.16530650971030389</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="7">
         <v>-0.36212721762928801</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="8">
         <v>0.91052557203555162</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="8">
         <v>0.79353787353382088</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17" s="6">
         <v>303</v>
       </c>
-      <c r="I17" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J17" s="9">
+      <c r="I17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17" s="6">
         <v>15</v>
       </c>
-      <c r="K17" s="10">
+      <c r="K17" s="7">
         <v>0.14686130335119069</v>
       </c>
-      <c r="L17" s="10">
+      <c r="L17" s="7">
         <v>-0.60059878249610599</v>
       </c>
-      <c r="M17" s="11">
+      <c r="M17" s="8">
         <v>0.55576759663725805</v>
       </c>
-      <c r="N17" s="11">
+      <c r="N17" s="8">
         <v>0.57980475176580526</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="9">
+    <row r="18" spans="1:14">
+      <c r="A18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="6">
         <v>185</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="7">
         <v>0.25060174035821531</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="7">
         <v>0.17348220117191221</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="7">
         <v>-0.50568982311881649</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="8">
         <v>0.8418595295706901</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="8">
         <v>0.73393463746147503</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="6">
         <v>88</v>
       </c>
-      <c r="I18" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J18" s="9">
+      <c r="I18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J18" s="6">
         <v>185</v>
       </c>
-      <c r="K18" s="10">
+      <c r="K18" s="7">
         <v>0.31342954317314381</v>
       </c>
-      <c r="L18" s="10">
+      <c r="L18" s="7">
         <v>-0.50568982311881661</v>
       </c>
-      <c r="M18" s="11">
+      <c r="M18" s="8">
         <v>0.85311640097664565</v>
       </c>
-      <c r="N18" s="11">
+      <c r="N18" s="8">
         <v>0.95431094976044217</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="9">
+    <row r="19" spans="1:14">
+      <c r="A19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="6">
         <v>190</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="7">
         <v>0.24537060667647489</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="7">
         <v>0.1679362847742101</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="7">
         <v>-0.50142636353316716</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="8">
         <v>0.82896078088314318</v>
       </c>
-      <c r="G19" s="11">
+      <c r="G19" s="8">
         <v>0.72245827409982866</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="6">
         <v>90</v>
       </c>
-      <c r="I19" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J19" s="9">
+      <c r="I19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J19" s="6">
         <v>190</v>
       </c>
-      <c r="K19" s="10">
+      <c r="K19" s="7">
         <v>0.31384001430488961</v>
       </c>
-      <c r="L19" s="10">
+      <c r="L19" s="7">
         <v>-0.50142636353316705</v>
       </c>
-      <c r="M19" s="11">
+      <c r="M19" s="8">
         <v>0.85328725207049227</v>
       </c>
-      <c r="N19" s="11">
+      <c r="N19" s="8">
         <v>0.95518607609333384</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="9">
+    <row r="20" spans="1:14">
+      <c r="A20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="6">
         <v>205</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="7">
         <v>0.24486212871211199</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="7">
         <v>0.16401508706126039</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="7">
         <v>-0.52030701141449676</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="8">
         <v>0.82150660921669216</v>
       </c>
-      <c r="G20" s="11">
+      <c r="G20" s="8">
         <v>0.71597230418551838</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="6">
         <v>88</v>
       </c>
-      <c r="I20" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J20" s="9">
+      <c r="I20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J20" s="6">
         <v>205</v>
       </c>
-      <c r="K20" s="10">
+      <c r="K20" s="7">
         <v>0.31325874997687381</v>
       </c>
-      <c r="L20" s="10">
+      <c r="L20" s="7">
         <v>-0.52030701141449698</v>
       </c>
-      <c r="M20" s="11">
+      <c r="M20" s="8">
         <v>0.84812138708062812</v>
       </c>
-      <c r="N20" s="11">
+      <c r="N20" s="8">
         <v>0.95135679386610617</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="9">
+    <row r="21" spans="1:14">
+      <c r="A21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="6">
         <v>180</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="7">
         <v>0.24159972602002819</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="7">
         <v>0.16912032391755721</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="7">
         <v>-0.50568982311881661</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="8">
         <v>0.82292383552150039</v>
       </c>
-      <c r="G21" s="11">
+      <c r="G21" s="8">
         <v>0.71641716031712066</v>
       </c>
-      <c r="H21" s="9">
+      <c r="H21" s="6">
         <v>90</v>
       </c>
-      <c r="I21" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J21" s="9">
+      <c r="I21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J21" s="6">
         <v>180</v>
       </c>
-      <c r="K21" s="10">
+      <c r="K21" s="7">
         <v>0.28786758039792232</v>
       </c>
-      <c r="L21" s="10">
+      <c r="L21" s="7">
         <v>-0.50568982311881649</v>
       </c>
-      <c r="M21" s="11">
+      <c r="M21" s="8">
         <v>0.80933607575666178</v>
       </c>
-      <c r="N21" s="11">
+      <c r="N21" s="8">
         <v>0.90279698107960948</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="9">
+    <row r="22" spans="1:14">
+      <c r="A22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="6">
         <v>45</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="7">
         <v>0.2355892298375715</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="7">
         <v>0.16054651435047579</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="7">
         <v>-0.43233207252818912</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="8">
         <v>0.85188872815601391</v>
       </c>
-      <c r="G22" s="11">
+      <c r="G22" s="8">
         <v>0.74746430279074727</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H22" s="6">
         <v>180</v>
       </c>
-      <c r="I22" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J22" s="9">
+      <c r="I22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J22" s="6">
         <v>45</v>
       </c>
-      <c r="K22" s="10">
+      <c r="K22" s="7">
         <v>0.2182386616072112</v>
       </c>
-      <c r="L22" s="10">
+      <c r="L22" s="7">
         <v>-0.4928382399899216</v>
       </c>
-      <c r="M22" s="11">
+      <c r="M22" s="8">
         <v>0.72268145688068519</v>
       </c>
-      <c r="N22" s="11">
+      <c r="N22" s="8">
         <v>0.7793790950301831</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="9">
+    <row r="23" spans="1:14">
+      <c r="A23" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="6">
         <v>35</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23" s="7">
         <v>0.23409132551294129</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="7">
         <v>0.1429964009717366</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="7">
         <v>-0.46339021847061312</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F23" s="8">
         <v>0.84648406044356506</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G23" s="8">
         <v>0.74371004232925442</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H23" s="6">
         <v>203</v>
       </c>
-      <c r="I23" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J23" s="9">
+      <c r="I23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J23" s="6">
         <v>35</v>
       </c>
-      <c r="K23" s="10">
+      <c r="K23" s="7">
         <v>0.1616351353373511</v>
       </c>
-      <c r="L23" s="10">
+      <c r="L23" s="7">
         <v>-0.53273772281591936</v>
       </c>
-      <c r="M23" s="11">
+      <c r="M23" s="8">
         <v>0.5943010981881256</v>
       </c>
-      <c r="N23" s="11">
+      <c r="N23" s="8">
         <v>0.62970164141703044</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="9">
+    <row r="24" spans="1:14">
+      <c r="A24" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="6">
         <v>175</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="7">
         <v>0.2225724632800854</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="7">
         <v>0.15165676474903461</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="7">
         <v>-0.50568982311881649</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="8">
         <v>0.77681130182030833</v>
       </c>
-      <c r="G24" s="11">
+      <c r="G24" s="8">
         <v>0.67505138334397741</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H24" s="6">
         <v>94</v>
       </c>
-      <c r="I24" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J24" s="9">
+      <c r="I24" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J24" s="6">
         <v>175</v>
       </c>
-      <c r="K24" s="10">
+      <c r="K24" s="7">
         <v>0.26806605677369499</v>
       </c>
-      <c r="L24" s="10">
+      <c r="L24" s="7">
         <v>-0.50568982311881649</v>
       </c>
-      <c r="M24" s="11">
+      <c r="M24" s="8">
         <v>0.77341052420662981</v>
       </c>
-      <c r="N24" s="11">
+      <c r="N24" s="8">
         <v>0.86148329820005787</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="9">
+    <row r="25" spans="1:14">
+      <c r="A25" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="6">
         <v>165</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25" s="7">
         <v>0.22085324003197379</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="7">
         <v>0.15141988608223961</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E25" s="7">
         <v>-0.50568982311881661</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F25" s="8">
         <v>0.77306372340959428</v>
       </c>
-      <c r="G25" s="11">
+      <c r="G25" s="8">
         <v>0.67452931767889113</v>
       </c>
-      <c r="H25" s="9">
+      <c r="H25" s="6">
         <v>104</v>
       </c>
-      <c r="I25" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J25" s="9">
+      <c r="I25" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J25" s="6">
         <v>165</v>
       </c>
-      <c r="K25" s="10">
+      <c r="K25" s="7">
         <v>0.23686630203637021</v>
       </c>
-      <c r="L25" s="10">
+      <c r="L25" s="7">
         <v>-0.50568982311881638</v>
       </c>
-      <c r="M25" s="11">
+      <c r="M25" s="8">
         <v>0.7167406391671105</v>
       </c>
-      <c r="N25" s="11">
+      <c r="N25" s="8">
         <v>0.79648910127275785</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B26" s="9">
+    <row r="26" spans="1:14">
+      <c r="A26" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="6">
         <v>75</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C26" s="7">
         <v>0.21825035430253381</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D26" s="7">
         <v>0.1525191814396738</v>
       </c>
-      <c r="E26" s="10">
+      <c r="E26" s="7">
         <v>-0.39609621181925181</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F26" s="8">
         <v>0.7943705632988014</v>
       </c>
-      <c r="G26" s="11">
+      <c r="G26" s="8">
         <v>0.69921944656724011</v>
       </c>
-      <c r="H26" s="9">
+      <c r="H26" s="6">
         <v>152</v>
       </c>
-      <c r="I26" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J26" s="9">
+      <c r="I26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J26" s="6">
         <v>75</v>
       </c>
-      <c r="K26" s="10">
+      <c r="K26" s="7">
         <v>0.1609331370431171</v>
       </c>
-      <c r="L26" s="10">
+      <c r="L26" s="7">
         <v>-0.54261264310499935</v>
       </c>
-      <c r="M26" s="11">
+      <c r="M26" s="8">
         <v>0.58374236274968161</v>
       </c>
-      <c r="N26" s="11">
+      <c r="N26" s="8">
         <v>0.61977902594605794</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" s="9">
+    <row r="27" spans="1:14">
+      <c r="A27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="6">
         <v>150</v>
       </c>
-      <c r="C27" s="10">
+      <c r="C27" s="7">
         <v>0.21640606778577981</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D27" s="7">
         <v>0.15626046668038679</v>
       </c>
-      <c r="E27" s="10">
+      <c r="E27" s="7">
         <v>-0.43806019679721619</v>
       </c>
-      <c r="F27" s="11">
+      <c r="F27" s="8">
         <v>0.76924076034854294</v>
       </c>
-      <c r="G27" s="11">
+      <c r="G27" s="8">
         <v>0.67774252978561056</v>
       </c>
-      <c r="H27" s="9">
+      <c r="H27" s="6">
         <v>120</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J27" s="9">
+      <c r="I27" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J27" s="6">
         <v>150</v>
       </c>
-      <c r="K27" s="10">
+      <c r="K27" s="7">
         <v>0.22972418991346191</v>
       </c>
-      <c r="L27" s="10">
+      <c r="L27" s="7">
         <v>-0.52865528649120752</v>
       </c>
-      <c r="M27" s="11">
+      <c r="M27" s="8">
         <v>0.70598829157951648</v>
       </c>
-      <c r="N27" s="11">
+      <c r="N27" s="8">
         <v>0.78975790644552746</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A28" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" s="9">
+    <row r="28" spans="1:14">
+      <c r="A28" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="6">
         <v>170</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C28" s="7">
         <v>0.21401210385381941</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="7">
         <v>0.1430078997643611</v>
       </c>
-      <c r="E28" s="10">
+      <c r="E28" s="7">
         <v>-0.50568982311881649</v>
       </c>
-      <c r="F28" s="11">
+      <c r="F28" s="8">
         <v>0.75697411677350135</v>
       </c>
-      <c r="G28" s="11">
+      <c r="G28" s="8">
         <v>0.65927277189328537</v>
       </c>
-      <c r="H28" s="9">
+      <c r="H28" s="6">
         <v>100</v>
       </c>
-      <c r="I28" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J28" s="9">
+      <c r="I28" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J28" s="6">
         <v>170</v>
       </c>
-      <c r="K28" s="10">
+      <c r="K28" s="7">
         <v>0.2492249258908377</v>
       </c>
-      <c r="L28" s="10">
+      <c r="L28" s="7">
         <v>-0.50568982311881649</v>
       </c>
-      <c r="M28" s="11">
+      <c r="M28" s="8">
         <v>0.73949734105008447</v>
       </c>
-      <c r="N28" s="11">
+      <c r="N28" s="8">
         <v>0.82365074892843304</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A29" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" s="9">
+    <row r="29" spans="1:14">
+      <c r="A29" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="6">
         <v>40</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C29" s="7">
         <v>0.21113602223331579</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D29" s="7">
         <v>0.13260516983827969</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29" s="7">
         <v>-0.43233207252818923</v>
       </c>
-      <c r="F29" s="11">
+      <c r="F29" s="8">
         <v>0.78358890406322024</v>
       </c>
-      <c r="G29" s="11">
+      <c r="G29" s="8">
         <v>0.68837330908189154</v>
       </c>
-      <c r="H29" s="9">
+      <c r="H29" s="6">
         <v>192</v>
       </c>
-      <c r="I29" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J29" s="9">
+      <c r="I29" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J29" s="6">
         <v>40</v>
       </c>
-      <c r="K29" s="10">
+      <c r="K29" s="7">
         <v>0.15168750740832609</v>
       </c>
-      <c r="L29" s="10">
+      <c r="L29" s="7">
         <v>-0.54543505454516539</v>
       </c>
-      <c r="M29" s="11">
+      <c r="M29" s="8">
         <v>0.56948519182010515</v>
       </c>
-      <c r="N29" s="11">
+      <c r="N29" s="8">
         <v>0.60554395817627804</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A30" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" s="9">
+    <row r="30" spans="1:14">
+      <c r="A30" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="6">
         <v>160</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C30" s="7">
         <v>0.2069379349954843</v>
       </c>
-      <c r="D30" s="10">
+      <c r="D30" s="7">
         <v>0.1427218274700788</v>
       </c>
-      <c r="E30" s="10">
+      <c r="E30" s="7">
         <v>-0.51408819009287232</v>
       </c>
-      <c r="F30" s="11">
+      <c r="F30" s="8">
         <v>0.7370678602235925</v>
       </c>
-      <c r="G30" s="11">
+      <c r="G30" s="8">
         <v>0.63873422344943265</v>
       </c>
-      <c r="H30" s="9">
+      <c r="H30" s="6">
         <v>108</v>
       </c>
-      <c r="I30" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J30" s="9">
+      <c r="I30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J30" s="6">
         <v>160</v>
       </c>
-      <c r="K30" s="10">
+      <c r="K30" s="7">
         <v>0.22274619041617891</v>
       </c>
-      <c r="L30" s="10">
+      <c r="L30" s="7">
         <v>-0.54145260569961207</v>
       </c>
-      <c r="M30" s="11">
+      <c r="M30" s="8">
         <v>0.689291277179921</v>
       </c>
-      <c r="N30" s="11">
+      <c r="N30" s="8">
         <v>0.76242019343454681</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A31" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B31" s="9">
+    <row r="31" spans="1:14">
+      <c r="A31" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="6">
         <v>50</v>
       </c>
-      <c r="C31" s="10">
+      <c r="C31" s="7">
         <v>0.205730530040134</v>
       </c>
-      <c r="D31" s="10">
+      <c r="D31" s="7">
         <v>0.1378757136049924</v>
       </c>
-      <c r="E31" s="10">
+      <c r="E31" s="7">
         <v>-0.44979013909864918</v>
       </c>
-      <c r="F31" s="11">
+      <c r="F31" s="8">
         <v>0.77126358954099306</v>
       </c>
-      <c r="G31" s="11">
+      <c r="G31" s="8">
         <v>0.67207219815074271</v>
       </c>
-      <c r="H31" s="9">
+      <c r="H31" s="6">
         <v>180</v>
       </c>
-      <c r="I31" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J31" s="9">
+      <c r="I31" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J31" s="6">
         <v>50</v>
       </c>
-      <c r="K31" s="10">
+      <c r="K31" s="7">
         <v>0.17185943855423069</v>
       </c>
-      <c r="L31" s="10">
+      <c r="L31" s="7">
         <v>-0.57640143394570598</v>
       </c>
-      <c r="M31" s="11">
+      <c r="M31" s="8">
         <v>0.6144450712116839</v>
       </c>
-      <c r="N31" s="11">
+      <c r="N31" s="8">
         <v>0.6563735782992256</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A32" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32" s="9">
+    <row r="32" spans="1:14">
+      <c r="A32" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="6">
         <v>80</v>
       </c>
-      <c r="C32" s="10">
+      <c r="C32" s="7">
         <v>0.20029955372614561</v>
       </c>
-      <c r="D32" s="10">
+      <c r="D32" s="7">
         <v>0.1359324753876292</v>
       </c>
-      <c r="E32" s="10">
+      <c r="E32" s="7">
         <v>-0.49912209282534409</v>
       </c>
-      <c r="F32" s="11">
+      <c r="F32" s="8">
         <v>0.7407325263138661</v>
       </c>
-      <c r="G32" s="11">
+      <c r="G32" s="8">
         <v>0.64450225002785844</v>
       </c>
-      <c r="H32" s="9">
+      <c r="H32" s="6">
         <v>147</v>
       </c>
-      <c r="I32" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J32" s="9">
+      <c r="I32" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J32" s="6">
         <v>80</v>
       </c>
-      <c r="K32" s="10">
+      <c r="K32" s="7">
         <v>0.16254460136501761</v>
       </c>
-      <c r="L32" s="10">
+      <c r="L32" s="7">
         <v>-0.45129811666150188</v>
       </c>
-      <c r="M32" s="11">
+      <c r="M32" s="8">
         <v>0.58435231286163392</v>
       </c>
-      <c r="N32" s="11">
+      <c r="N32" s="8">
         <v>0.61858558738179181</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A33" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B33" s="9">
+    <row r="33" spans="1:14">
+      <c r="A33" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="6">
         <v>60</v>
       </c>
-      <c r="C33" s="10">
+      <c r="C33" s="7">
         <v>0.19887345934488129</v>
       </c>
-      <c r="D33" s="10">
+      <c r="D33" s="7">
         <v>0.13506488298047301</v>
       </c>
-      <c r="E33" s="10">
+      <c r="E33" s="7">
         <v>-0.49467602987385573</v>
       </c>
-      <c r="F33" s="11">
+      <c r="F33" s="8">
         <v>0.74852674899881266</v>
       </c>
-      <c r="G33" s="11">
+      <c r="G33" s="8">
         <v>0.64523383182404181</v>
       </c>
-      <c r="H33" s="9">
+      <c r="H33" s="6">
         <v>152</v>
       </c>
-      <c r="I33" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J33" s="9">
+      <c r="I33" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J33" s="6">
         <v>60</v>
       </c>
-      <c r="K33" s="10">
+      <c r="K33" s="7">
         <v>0.1439870599793556</v>
       </c>
-      <c r="L33" s="10">
+      <c r="L33" s="7">
         <v>-0.63445152043385189</v>
       </c>
-      <c r="M33" s="11">
+      <c r="M33" s="8">
         <v>0.54891115011122338</v>
       </c>
-      <c r="N33" s="11">
+      <c r="N33" s="8">
         <v>0.57749859452898955</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A34" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B34" s="9">
+    <row r="34" spans="1:14">
+      <c r="A34" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="6">
         <v>145</v>
       </c>
-      <c r="C34" s="10">
+      <c r="C34" s="7">
         <v>0.19762441749424481</v>
       </c>
-      <c r="D34" s="10">
+      <c r="D34" s="7">
         <v>0.14023074760359869</v>
       </c>
-      <c r="E34" s="10">
+      <c r="E34" s="7">
         <v>-0.47051017796388261</v>
       </c>
-      <c r="F34" s="11">
+      <c r="F34" s="8">
         <v>0.72204009835323202</v>
       </c>
-      <c r="G34" s="11">
+      <c r="G34" s="8">
         <v>0.63330101572230213</v>
       </c>
-      <c r="H34" s="9">
+      <c r="H34" s="6">
         <v>127</v>
       </c>
-      <c r="I34" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J34" s="9">
+      <c r="I34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J34" s="6">
         <v>145</v>
       </c>
-      <c r="K34" s="10">
+      <c r="K34" s="7">
         <v>0.19664372795472351</v>
       </c>
-      <c r="L34" s="10">
+      <c r="L34" s="7">
         <v>-0.58267984171433285</v>
       </c>
-      <c r="M34" s="11">
+      <c r="M34" s="8">
         <v>0.64235727381033325</v>
       </c>
-      <c r="N34" s="11">
+      <c r="N34" s="8">
         <v>0.71360288614616207</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A35" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B35" s="9">
+    <row r="35" spans="1:14">
+      <c r="A35" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="6">
         <v>70</v>
       </c>
-      <c r="C35" s="10">
+      <c r="C35" s="7">
         <v>0.1951251965774092</v>
       </c>
-      <c r="D35" s="10">
+      <c r="D35" s="7">
         <v>0.1312240239502778</v>
       </c>
-      <c r="E35" s="10">
+      <c r="E35" s="7">
         <v>-0.44836263853328251</v>
       </c>
-      <c r="F35" s="11">
+      <c r="F35" s="8">
         <v>0.733301233653748</v>
       </c>
-      <c r="G35" s="11">
+      <c r="G35" s="8">
         <v>0.63752762426273024</v>
       </c>
-      <c r="H35" s="9">
+      <c r="H35" s="6">
         <v>150</v>
       </c>
-      <c r="I35" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J35" s="9">
+      <c r="I35" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J35" s="6">
         <v>70</v>
       </c>
-      <c r="K35" s="10">
+      <c r="K35" s="7">
         <v>0.1259741566557819</v>
       </c>
-      <c r="L35" s="10">
+      <c r="L35" s="7">
         <v>-0.6263988126991562</v>
       </c>
-      <c r="M35" s="11">
+      <c r="M35" s="8">
         <v>0.50446431272255454</v>
       </c>
-      <c r="N35" s="11">
+      <c r="N35" s="8">
         <v>0.53047357113694882</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A36" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B36" s="9">
+    <row r="36" spans="1:14">
+      <c r="A36" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="6">
         <v>155</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C36" s="7">
         <v>0.19458773374100419</v>
       </c>
-      <c r="D36" s="10">
+      <c r="D36" s="7">
         <v>0.1335439183433931</v>
       </c>
-      <c r="E36" s="10">
+      <c r="E36" s="7">
         <v>-0.52591679182476492</v>
       </c>
-      <c r="F36" s="11">
+      <c r="F36" s="8">
         <v>0.70705694663683982</v>
       </c>
-      <c r="G36" s="11">
+      <c r="G36" s="8">
         <v>0.60975124156230276</v>
       </c>
-      <c r="H36" s="9">
+      <c r="H36" s="6">
         <v>120</v>
       </c>
-      <c r="I36" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J36" s="9">
+      <c r="I36" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J36" s="6">
         <v>155</v>
       </c>
-      <c r="K36" s="10">
+      <c r="K36" s="7">
         <v>0.2026130543549802</v>
       </c>
-      <c r="L36" s="10">
+      <c r="L36" s="7">
         <v>-0.52761019663010056</v>
       </c>
-      <c r="M36" s="11">
+      <c r="M36" s="8">
         <v>0.65071052690949083</v>
       </c>
-      <c r="N36" s="11">
+      <c r="N36" s="8">
         <v>0.71714823294854746</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A37" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B37" s="9">
+    <row r="37" spans="1:14">
+      <c r="A37" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="6">
         <v>85</v>
       </c>
-      <c r="C37" s="10">
+      <c r="C37" s="7">
         <v>0.19435349833509269</v>
       </c>
-      <c r="D37" s="10">
+      <c r="D37" s="7">
         <v>0.12735824666379969</v>
       </c>
-      <c r="E37" s="10">
+      <c r="E37" s="7">
         <v>-0.47137699597667942</v>
       </c>
-      <c r="F37" s="11">
+      <c r="F37" s="8">
         <v>0.72542744709112461</v>
       </c>
-      <c r="G37" s="11">
+      <c r="G37" s="8">
         <v>0.6293070198584082</v>
       </c>
-      <c r="H37" s="9">
+      <c r="H37" s="6">
         <v>145</v>
       </c>
-      <c r="I37" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J37" s="9">
+      <c r="I37" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J37" s="6">
         <v>85</v>
       </c>
-      <c r="K37" s="10">
+      <c r="K37" s="7">
         <v>0.16439830812003689</v>
       </c>
-      <c r="L37" s="10">
+      <c r="L37" s="7">
         <v>-0.49099686300930551</v>
       </c>
-      <c r="M37" s="11">
+      <c r="M37" s="8">
         <v>0.58784960701520572</v>
       </c>
-      <c r="N37" s="11">
+      <c r="N37" s="8">
         <v>0.62172296930976612</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A38" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B38" s="9">
+    <row r="38" spans="1:14">
+      <c r="A38" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="6">
         <v>65</v>
       </c>
-      <c r="C38" s="10">
+      <c r="C38" s="7">
         <v>0.18520879978228949</v>
       </c>
-      <c r="D38" s="10">
+      <c r="D38" s="7">
         <v>0.1225748161532991</v>
       </c>
-      <c r="E38" s="10">
+      <c r="E38" s="7">
         <v>-0.49678250789046252</v>
       </c>
-      <c r="F38" s="11">
+      <c r="F38" s="8">
         <v>0.70736388235892522</v>
       </c>
-      <c r="G38" s="11">
+      <c r="G38" s="8">
         <v>0.60667839345875207</v>
       </c>
-      <c r="H38" s="9">
+      <c r="H38" s="6">
         <v>142</v>
       </c>
-      <c r="I38" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J38" s="9">
+      <c r="I38" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J38" s="6">
         <v>65</v>
       </c>
-      <c r="K38" s="10">
+      <c r="K38" s="7">
         <v>0.10356477626233281</v>
       </c>
-      <c r="L38" s="10">
+      <c r="L38" s="7">
         <v>-0.6935059922183181</v>
       </c>
-      <c r="M38" s="11">
+      <c r="M38" s="8">
         <v>0.45238834227928632</v>
       </c>
-      <c r="N38" s="11">
+      <c r="N38" s="8">
         <v>0.47166354446420838</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A39" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B39" s="9">
+    <row r="39" spans="1:14">
+      <c r="A39" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="6">
         <v>55</v>
       </c>
-      <c r="C39" s="10">
+      <c r="C39" s="7">
         <v>0.18355332482347511</v>
       </c>
-      <c r="D39" s="10">
+      <c r="D39" s="7">
         <v>0.1151393261262996</v>
       </c>
-      <c r="E39" s="10">
+      <c r="E39" s="7">
         <v>-0.48954796901973691</v>
       </c>
-      <c r="F39" s="11">
+      <c r="F39" s="8">
         <v>0.70553392535720882</v>
       </c>
-      <c r="G39" s="11">
+      <c r="G39" s="8">
         <v>0.60503226223130879</v>
       </c>
-      <c r="H39" s="9">
+      <c r="H39" s="6">
         <v>166</v>
       </c>
-      <c r="I39" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J39" s="9">
+      <c r="I39" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J39" s="6">
         <v>55</v>
       </c>
-      <c r="K39" s="10">
+      <c r="K39" s="7">
         <v>0.1130247914139737</v>
       </c>
-      <c r="L39" s="10">
+      <c r="L39" s="7">
         <v>-0.69260990700369285</v>
       </c>
-      <c r="M39" s="11">
+      <c r="M39" s="8">
         <v>0.47600884735196197</v>
       </c>
-      <c r="N39" s="11">
+      <c r="N39" s="8">
         <v>0.50096596194640186</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A40" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B40" s="9">
+    <row r="40" spans="1:14">
+      <c r="A40" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="6">
         <v>105</v>
       </c>
-      <c r="C40" s="10">
+      <c r="C40" s="7">
         <v>0.17961341304638931</v>
       </c>
-      <c r="D40" s="10">
+      <c r="D40" s="7">
         <v>0.10865392490435501</v>
       </c>
-      <c r="E40" s="10">
+      <c r="E40" s="7">
         <v>-0.63158946404792171</v>
       </c>
-      <c r="F40" s="11">
+      <c r="F40" s="8">
         <v>0.68613786769651108</v>
       </c>
-      <c r="G40" s="11">
+      <c r="G40" s="8">
         <v>0.587477157583988</v>
       </c>
-      <c r="H40" s="9">
+      <c r="H40" s="6">
         <v>122</v>
       </c>
-      <c r="I40" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J40" s="9">
+      <c r="I40" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J40" s="6">
         <v>105</v>
       </c>
-      <c r="K40" s="10">
+      <c r="K40" s="7">
         <v>0.11850230456868641</v>
       </c>
-      <c r="L40" s="10">
+      <c r="L40" s="7">
         <v>-0.59913583989247432</v>
       </c>
-      <c r="M40" s="11">
+      <c r="M40" s="8">
         <v>0.48355245730450408</v>
       </c>
-      <c r="N40" s="11">
+      <c r="N40" s="8">
         <v>0.51902967678095568</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A41" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B41" s="9">
+    <row r="41" spans="1:14">
+      <c r="A41" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" s="6">
         <v>140</v>
       </c>
-      <c r="C41" s="10">
+      <c r="C41" s="7">
         <v>0.17271554684207449</v>
       </c>
-      <c r="D41" s="10">
+      <c r="D41" s="7">
         <v>0.116938438252743</v>
       </c>
-      <c r="E41" s="10">
+      <c r="E41" s="7">
         <v>-0.52804312955931765</v>
       </c>
-      <c r="F41" s="11">
+      <c r="F41" s="8">
         <v>0.65954504679667414</v>
       </c>
-      <c r="G41" s="11">
+      <c r="G41" s="8">
         <v>0.57261080094911332</v>
       </c>
-      <c r="H41" s="9">
+      <c r="H41" s="6">
         <v>129</v>
       </c>
-      <c r="I41" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J41" s="9">
+      <c r="I41" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J41" s="6">
         <v>140</v>
       </c>
-      <c r="K41" s="10">
+      <c r="K41" s="7">
         <v>0.16165709434474601</v>
       </c>
-      <c r="L41" s="10">
+      <c r="L41" s="7">
         <v>-0.60690774115762913</v>
       </c>
-      <c r="M41" s="11">
+      <c r="M41" s="8">
         <v>0.57235219787676683</v>
       </c>
-      <c r="N41" s="11">
+      <c r="N41" s="8">
         <v>0.63031026355270314</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A42" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B42" s="9">
+    <row r="42" spans="1:14">
+      <c r="A42" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="6">
         <v>110</v>
       </c>
-      <c r="C42" s="10">
+      <c r="C42" s="7">
         <v>0.17101475549018749</v>
       </c>
-      <c r="D42" s="10">
+      <c r="D42" s="7">
         <v>0.10294006571547019</v>
       </c>
-      <c r="E42" s="10">
+      <c r="E42" s="7">
         <v>-0.63685296023997662</v>
       </c>
-      <c r="F42" s="11">
+      <c r="F42" s="8">
         <v>0.66155928742529835</v>
       </c>
-      <c r="G42" s="11">
+      <c r="G42" s="8">
         <v>0.56746017426570761</v>
       </c>
-      <c r="H42" s="9">
+      <c r="H42" s="6">
         <v>128</v>
       </c>
-      <c r="I42" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J42" s="9">
+      <c r="I42" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J42" s="6">
         <v>110</v>
       </c>
-      <c r="K42" s="10">
+      <c r="K42" s="7">
         <v>0.12815271700543801</v>
       </c>
-      <c r="L42" s="10">
+      <c r="L42" s="7">
         <v>-0.57675023431353722</v>
       </c>
-      <c r="M42" s="11">
+      <c r="M42" s="8">
         <v>0.50412825559419416</v>
       </c>
-      <c r="N42" s="11">
+      <c r="N42" s="8">
         <v>0.54422108755569754</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A43" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B43" s="9">
+    <row r="43" spans="1:14">
+      <c r="A43" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" s="6">
         <v>100</v>
       </c>
-      <c r="C43" s="10">
+      <c r="C43" s="7">
         <v>0.16945362360001329</v>
       </c>
-      <c r="D43" s="10">
+      <c r="D43" s="7">
         <v>0.1009432567389312</v>
       </c>
-      <c r="E43" s="10">
+      <c r="E43" s="7">
         <v>-0.58404892033710121</v>
       </c>
-      <c r="F43" s="11">
+      <c r="F43" s="8">
         <v>0.65646246202734204</v>
       </c>
-      <c r="G43" s="11">
+      <c r="G43" s="8">
         <v>0.55900447444436185</v>
       </c>
-      <c r="H43" s="9">
+      <c r="H43" s="6">
         <v>130</v>
       </c>
-      <c r="I43" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J43" s="9">
+      <c r="I43" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J43" s="6">
         <v>100</v>
       </c>
-      <c r="K43" s="10">
+      <c r="K43" s="7">
         <v>0.11032404948611201</v>
       </c>
-      <c r="L43" s="10">
+      <c r="L43" s="7">
         <v>-0.54366175524614557</v>
       </c>
-      <c r="M43" s="11">
+      <c r="M43" s="8">
         <v>0.46554555602933162</v>
       </c>
-      <c r="N43" s="11">
+      <c r="N43" s="8">
         <v>0.49431920399869911</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A44" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B44" s="9">
+    <row r="44" spans="1:14">
+      <c r="A44" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="6">
         <v>135</v>
       </c>
-      <c r="C44" s="10">
+      <c r="C44" s="7">
         <v>0.1684381715775152</v>
       </c>
-      <c r="D44" s="10">
+      <c r="D44" s="7">
         <v>0.1121269001114118</v>
       </c>
-      <c r="E44" s="10">
+      <c r="E44" s="7">
         <v>-0.53943363004376343</v>
       </c>
-      <c r="F44" s="11">
+      <c r="F44" s="8">
         <v>0.64843511162571077</v>
       </c>
-      <c r="G44" s="11">
+      <c r="G44" s="8">
         <v>0.56256813272475403</v>
       </c>
-      <c r="H44" s="9">
+      <c r="H44" s="6">
         <v>136</v>
       </c>
-      <c r="I44" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J44" s="9">
+      <c r="I44" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J44" s="6">
         <v>135</v>
       </c>
-      <c r="K44" s="10">
+      <c r="K44" s="7">
         <v>0.1598114877518699</v>
       </c>
-      <c r="L44" s="10">
+      <c r="L44" s="7">
         <v>-0.58369234257759295</v>
       </c>
-      <c r="M44" s="11">
+      <c r="M44" s="8">
         <v>0.56916764428265465</v>
       </c>
-      <c r="N44" s="11">
+      <c r="N44" s="8">
         <v>0.62529078342770428</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A45" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B45" s="9">
+    <row r="45" spans="1:14">
+      <c r="A45" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" s="6">
         <v>95</v>
       </c>
-      <c r="C45" s="10">
+      <c r="C45" s="7">
         <v>0.1657641495269182</v>
       </c>
-      <c r="D45" s="10">
+      <c r="D45" s="7">
         <v>9.9301016327224101E-2</v>
       </c>
-      <c r="E45" s="10">
+      <c r="E45" s="7">
         <v>-0.56887543384767425</v>
       </c>
-      <c r="F45" s="11">
+      <c r="F45" s="8">
         <v>0.64655520689051194</v>
       </c>
-      <c r="G45" s="11">
+      <c r="G45" s="8">
         <v>0.55145622353076695</v>
       </c>
-      <c r="H45" s="9">
+      <c r="H45" s="6">
         <v>137</v>
       </c>
-      <c r="I45" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J45" s="9">
+      <c r="I45" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J45" s="6">
         <v>95</v>
       </c>
-      <c r="K45" s="10">
+      <c r="K45" s="7">
         <v>0.1192112635978162</v>
       </c>
-      <c r="L45" s="10">
+      <c r="L45" s="7">
         <v>-0.55605479995119611</v>
       </c>
-      <c r="M45" s="11">
+      <c r="M45" s="8">
         <v>0.48573892003918362</v>
       </c>
-      <c r="N45" s="11">
+      <c r="N45" s="8">
         <v>0.51345191192816242</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A46" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B46" s="9">
+    <row r="46" spans="1:14">
+      <c r="A46" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="6">
         <v>90</v>
       </c>
-      <c r="C46" s="10">
+      <c r="C46" s="7">
         <v>0.1644738958959415</v>
       </c>
-      <c r="D46" s="10">
+      <c r="D46" s="7">
         <v>9.6216585560279233E-2</v>
       </c>
-      <c r="E46" s="10">
+      <c r="E46" s="7">
         <v>-0.48598231500882272</v>
       </c>
-      <c r="F46" s="11">
+      <c r="F46" s="8">
         <v>0.64312350668818952</v>
       </c>
-      <c r="G46" s="11">
+      <c r="G46" s="8">
         <v>0.55407521689953987</v>
       </c>
-      <c r="H46" s="9">
+      <c r="H46" s="6">
         <v>151</v>
       </c>
-      <c r="I46" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J46" s="9">
+      <c r="I46" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J46" s="6">
         <v>90</v>
       </c>
-      <c r="K46" s="10">
+      <c r="K46" s="7">
         <v>0.1331413734815006</v>
       </c>
-      <c r="L46" s="10">
+      <c r="L46" s="7">
         <v>-0.54413621037526516</v>
       </c>
-      <c r="M46" s="11">
+      <c r="M46" s="8">
         <v>0.51739589589398649</v>
       </c>
-      <c r="N46" s="11">
+      <c r="N46" s="8">
         <v>0.54858281817414767</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A47" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B47" s="9">
+    <row r="47" spans="1:14">
+      <c r="A47" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" s="6">
         <v>125</v>
       </c>
-      <c r="C47" s="10">
+      <c r="C47" s="7">
         <v>0.16233520752870079</v>
       </c>
-      <c r="D47" s="10">
+      <c r="D47" s="7">
         <v>0.10177993316505619</v>
       </c>
-      <c r="E47" s="10">
+      <c r="E47" s="7">
         <v>-0.6193521990413835</v>
       </c>
-      <c r="F47" s="11">
+      <c r="F47" s="8">
         <v>0.63676782591513881</v>
       </c>
-      <c r="G47" s="11">
+      <c r="G47" s="8">
         <v>0.54568865927413823</v>
       </c>
-      <c r="H47" s="9">
+      <c r="H47" s="6">
         <v>128</v>
       </c>
-      <c r="I47" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J47" s="9">
+      <c r="I47" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J47" s="6">
         <v>125</v>
       </c>
-      <c r="K47" s="10">
+      <c r="K47" s="7">
         <v>0.13588748802305381</v>
       </c>
-      <c r="L47" s="10">
+      <c r="L47" s="7">
         <v>-0.54830188201460739</v>
       </c>
-      <c r="M47" s="11">
+      <c r="M47" s="8">
         <v>0.51995809113375346</v>
       </c>
-      <c r="N47" s="11">
+      <c r="N47" s="8">
         <v>0.56602007364199214</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A48" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B48" s="9">
+    <row r="48" spans="1:14">
+      <c r="A48" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" s="6">
         <v>115</v>
       </c>
-      <c r="C48" s="10">
+      <c r="C48" s="7">
         <v>0.1622094527206783</v>
       </c>
-      <c r="D48" s="10">
+      <c r="D48" s="7">
         <v>9.7130916113564281E-2</v>
       </c>
-      <c r="E48" s="10">
+      <c r="E48" s="7">
         <v>-0.60283479372699256</v>
       </c>
-      <c r="F48" s="11">
+      <c r="F48" s="8">
         <v>0.63721582457643289</v>
       </c>
-      <c r="G48" s="11">
+      <c r="G48" s="8">
         <v>0.54465825930190492</v>
       </c>
-      <c r="H48" s="9">
+      <c r="H48" s="6">
         <v>126</v>
       </c>
-      <c r="I48" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J48" s="9">
+      <c r="I48" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J48" s="6">
         <v>115</v>
       </c>
-      <c r="K48" s="10">
+      <c r="K48" s="7">
         <v>0.1087942317683577</v>
       </c>
-      <c r="L48" s="10">
+      <c r="L48" s="7">
         <v>-0.56738760961398649</v>
       </c>
-      <c r="M48" s="11">
+      <c r="M48" s="8">
         <v>0.46090162669485002</v>
       </c>
-      <c r="N48" s="11">
+      <c r="N48" s="8">
         <v>0.4976654943847274</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A49" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B49" s="9">
+    <row r="49" spans="1:14">
+      <c r="A49" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="6">
         <v>130</v>
       </c>
-      <c r="C49" s="10">
+      <c r="C49" s="7">
         <v>0.14992994838479981</v>
       </c>
-      <c r="D49" s="10">
+      <c r="D49" s="7">
         <v>9.2551265093429924E-2</v>
       </c>
-      <c r="E49" s="10">
+      <c r="E49" s="7">
         <v>-0.62923150276685402</v>
       </c>
-      <c r="F49" s="11">
+      <c r="F49" s="8">
         <v>0.60237921686561047</v>
       </c>
-      <c r="G49" s="11">
+      <c r="G49" s="8">
         <v>0.51607266183436529</v>
       </c>
-      <c r="H49" s="9">
+      <c r="H49" s="6">
         <v>131</v>
       </c>
-      <c r="I49" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J49" s="9">
+      <c r="I49" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J49" s="6">
         <v>130</v>
       </c>
-      <c r="K49" s="10">
+      <c r="K49" s="7">
         <v>0.13148463377062281</v>
       </c>
-      <c r="L49" s="10">
+      <c r="L49" s="7">
         <v>-0.56013593361616376</v>
       </c>
-      <c r="M49" s="11">
+      <c r="M49" s="8">
         <v>0.51017624946824258</v>
       </c>
-      <c r="N49" s="11">
+      <c r="N49" s="8">
         <v>0.55603710039115761</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A50" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B50" s="9">
+    <row r="50" spans="1:14">
+      <c r="A50" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B50" s="6">
         <v>120</v>
       </c>
-      <c r="C50" s="10">
+      <c r="C50" s="7">
         <v>0.1494505567664077</v>
       </c>
-      <c r="D50" s="10">
+      <c r="D50" s="7">
         <v>8.2750002045469451E-2</v>
       </c>
-      <c r="E50" s="10">
+      <c r="E50" s="7">
         <v>-0.58626067421049211</v>
       </c>
-      <c r="F50" s="11">
+      <c r="F50" s="8">
         <v>0.60092246722712583</v>
       </c>
-      <c r="G50" s="11">
+      <c r="G50" s="8">
         <v>0.51402480501089098</v>
       </c>
-      <c r="H50" s="9">
+      <c r="H50" s="6">
         <v>134</v>
       </c>
-      <c r="I50" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J50" s="9">
+      <c r="I50" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J50" s="6">
         <v>120</v>
       </c>
-      <c r="K50" s="10">
+      <c r="K50" s="7">
         <v>0.1198750338392771</v>
       </c>
-      <c r="L50" s="10">
+      <c r="L50" s="7">
         <v>-0.56033114375598614</v>
       </c>
-      <c r="M50" s="11">
+      <c r="M50" s="8">
         <v>0.48517974739188852</v>
       </c>
-      <c r="N50" s="11">
+      <c r="N50" s="8">
         <v>0.52523978942467109</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A51" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B51" s="9">
+    <row r="51" spans="1:14">
+      <c r="A51" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" s="6">
         <v>5</v>
       </c>
-      <c r="C51" s="10">
+      <c r="C51" s="7">
         <v>0.14121389502704809</v>
       </c>
-      <c r="D51" s="10">
+      <c r="D51" s="7">
         <v>8.1855396401760094E-2</v>
       </c>
-      <c r="E51" s="10">
+      <c r="E51" s="7">
         <v>-0.5024808995224519</v>
       </c>
-      <c r="F51" s="11">
+      <c r="F51" s="8">
         <v>0.59167286796060103</v>
       </c>
-      <c r="G51" s="11">
+      <c r="G51" s="8">
         <v>0.48446832252505773</v>
       </c>
-      <c r="H51" s="9">
+      <c r="H51" s="6">
         <v>557</v>
       </c>
-      <c r="I51" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J51" s="9">
+      <c r="I51" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J51" s="6">
         <v>5</v>
       </c>
-      <c r="K51" s="10">
+      <c r="K51" s="7">
         <v>4.6339720426293203E-2</v>
       </c>
-      <c r="L51" s="10">
+      <c r="L51" s="7">
         <v>-0.71784589168319646</v>
       </c>
-      <c r="M51" s="11">
+      <c r="M51" s="8">
         <v>0.31532528685483763</v>
       </c>
-      <c r="N51" s="11">
+      <c r="N51" s="8">
         <v>0.32127170864283627</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A52" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B52" s="9">
+    <row r="52" spans="1:14">
+      <c r="A52" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="6">
         <v>10</v>
       </c>
-      <c r="C52" s="10">
+      <c r="C52" s="7">
         <v>0.13667233181637031</v>
       </c>
-      <c r="D52" s="10">
+      <c r="D52" s="7">
         <v>7.896873250548242E-2</v>
       </c>
-      <c r="E52" s="10">
+      <c r="E52" s="7">
         <v>-0.50754707161196988</v>
       </c>
-      <c r="F52" s="11">
+      <c r="F52" s="8">
         <v>0.58056802772238347</v>
       </c>
-      <c r="G52" s="11">
+      <c r="G52" s="8">
         <v>0.48391483473350672</v>
       </c>
-      <c r="H52" s="9">
+      <c r="H52" s="6">
         <v>401</v>
       </c>
-      <c r="I52" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J52" s="9">
+      <c r="I52" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J52" s="6">
         <v>10</v>
       </c>
-      <c r="K52" s="10">
+      <c r="K52" s="7">
         <v>3.4265799815172748E-2</v>
       </c>
-      <c r="L52" s="10">
+      <c r="L52" s="7">
         <v>-0.70374279778188631</v>
       </c>
-      <c r="M52" s="11">
+      <c r="M52" s="8">
         <v>0.28146541413174508</v>
       </c>
-      <c r="N52" s="11">
+      <c r="N52" s="8">
         <v>0.28554271310432172</v>
       </c>
     </row>
@@ -2854,42 +2850,42 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="11.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="6">
         <v>0.3457671090136043</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="6">
         <v>-0.81659848664579748</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="6">
         <v>0.79451975814654963</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="6">
         <v>1.0186417049537391</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new file:   TQQQ_MA/TQQQ_MA_AGG4m.xlsx 	modified:   "TQQQ_MA/TQQQ_MA_AGG4m\354\265\234\354\242\205.py" 	modified:   TQQQ_MA/TQQQ_Results.xlsx 	new file:   Trading/Binance_MA/Bybit_auto_trend.py 	new file:   Trading/Binance_MA/Upbit_auto_trend.py 	new file:   Trading/Binance_MA/binance_auto_rsi_10_4.py 	new file:   Trading/Binance_MA/binance_auto_trend.py 	new file:   Trading/Binance_MA/binance_auto_trend_10_2.py 	new file:   Trading/Upbit_MA/Upbit_auto_trend.py
</commit_message>
<xml_diff>
--- a/TQQQ_MA/TQQQ_Results.xlsx
+++ b/TQQQ_MA/TQQQ_Results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilpus\PythonProjects\git_folder\TQQQ_MA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilpus\Desktop\git_folder\TQQQ_MA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E105CC45-9383-45F9-A7A9-672CA1836C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9014BEE3-3B3E-4E89-9C14-9C1934005D6F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="345" yWindow="240" windowWidth="20310" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="16">
   <si>
     <t>Model</t>
   </si>
@@ -67,6 +67,10 @@
   <si>
     <t>TQQQ BH</t>
   </si>
+  <si>
+    <t>TQQQ MA+AGG</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -75,7 +79,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,6 +103,15 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -149,7 +162,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -158,14 +171,22 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="백분율" xfId="1" builtinId="5"/>
@@ -472,15 +493,17 @@
   <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="3" max="3" width="9" style="6" customWidth="1"/>
-    <col min="4" max="4" width="11" style="6" customWidth="1"/>
-    <col min="5" max="5" width="9" style="6" customWidth="1"/>
+    <col min="1" max="1" width="20.375" customWidth="1"/>
+    <col min="3" max="3" width="9" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11" style="4" customWidth="1"/>
+    <col min="5" max="5" width="9" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10.625" customWidth="1"/>
+    <col min="9" max="9" width="15.125" customWidth="1"/>
     <col min="11" max="12" width="9" style="3" customWidth="1"/>
   </cols>
   <sheetData>
@@ -491,13 +514,13 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -529,13 +552,13 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="4">
+      <c r="A2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="6">
         <v>20</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="7">
         <v>0.33110387391737789</v>
       </c>
       <c r="D2" s="7">
@@ -544,2237 +567,2238 @@
       <c r="E2" s="7">
         <v>-0.29128415918770822</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="6">
         <v>1.1198138592348541</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="6">
         <v>1.007628572748144</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="6">
         <v>249</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="4">
+      <c r="I2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="6">
         <v>20</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2" s="8">
         <v>0.29522618674067869</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2" s="8">
         <v>-0.42747532803057159</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2" s="6">
         <v>0.89646209446052616</v>
       </c>
-      <c r="N2" s="4">
+      <c r="N2" s="6">
         <v>0.97784014156018706</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3">
+      <c r="A3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="9">
         <v>225</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="10">
         <v>0.29755158040884488</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="10">
         <v>0.208131307840008</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="10">
         <v>-0.5009499593972806</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="9">
         <v>0.95228746539363307</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="9">
         <v>0.83965903971862221</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="9">
         <v>82</v>
       </c>
-      <c r="I3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3">
+      <c r="I3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="9">
         <v>225</v>
       </c>
-      <c r="K3" s="3">
+      <c r="K3" s="11">
         <v>0.35068097319622699</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="11">
         <v>-0.50094995939728038</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="9">
         <v>0.91507861673457325</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="9">
         <v>1.0296034674458041</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
+      <c r="A4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="9">
         <v>235</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="10">
         <v>0.30000475945176591</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="10">
         <v>0.203077827417494</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="10">
         <v>-0.5009499593972806</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="9">
         <v>0.95417939140983843</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="9">
         <v>0.84322824451249134</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="9">
         <v>76</v>
       </c>
-      <c r="I4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4">
+      <c r="I4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="9">
         <v>235</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="11">
         <v>0.33749338538468859</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="11">
         <v>-0.5009499593972806</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="9">
         <v>0.88935029493728857</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="9">
         <v>0.99950349411118722</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5">
+      <c r="A5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="9">
         <v>240</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="10">
         <v>0.29869264766255671</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="10">
         <v>0.20285139377653899</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="10">
         <v>-0.50094995939728071</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="9">
         <v>0.95076197732725876</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="9">
         <v>0.8413211975979864</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="9">
         <v>76</v>
       </c>
-      <c r="I5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5">
+      <c r="I5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="9">
         <v>240</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="11">
         <v>0.32223275309435961</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5" s="11">
         <v>-0.5009499593972806</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="9">
         <v>0.8613272864710132</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="9">
         <v>0.96406569265673314</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6">
+      <c r="A6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="9">
         <v>230</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="10">
         <v>0.29804919060468271</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="10">
         <v>0.2017644572126942</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="10">
         <v>-0.50094995939728049</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="9">
         <v>0.95067609031876321</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="9">
         <v>0.83834635009205583</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="9">
         <v>78</v>
       </c>
-      <c r="I6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6">
+      <c r="I6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="9">
         <v>230</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="11">
         <v>0.340278606308831</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="11">
         <v>-0.5009499593972806</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="9">
         <v>0.89582223291914342</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="9">
         <v>1.0095224121781179</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7">
+      <c r="A7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="9">
         <v>25</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="10">
         <v>0.2911273627228439</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="10">
         <v>0.20067692224625169</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="10">
         <v>-0.38563801364223033</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="9">
         <v>0.99892146993008524</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="9">
         <v>0.87098853137440169</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="9">
         <v>212</v>
       </c>
-      <c r="I7" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7">
+      <c r="I7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="9">
         <v>25</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="11">
         <v>0.19044467252353309</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="11">
         <v>-0.63669992419152988</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="9">
         <v>0.66219329675414695</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="9">
         <v>0.69945589721895973</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8">
+      <c r="A8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="9">
         <v>30</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="10">
         <v>0.29961204155636861</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="10">
         <v>0.19378797989136931</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="10">
         <v>-0.515108081946829</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="9">
         <v>1.0122662405908169</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="9">
         <v>0.89326963815975591</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="9">
         <v>198</v>
       </c>
-      <c r="I8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8">
+      <c r="I8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="9">
         <v>30</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8" s="11">
         <v>0.212026314520398</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8" s="11">
         <v>-0.62585436868169719</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="9">
         <v>0.70768428773611691</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="9">
         <v>0.75311607813465831</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9">
+      <c r="A9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="9">
         <v>220</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="10">
         <v>0.27939401081663018</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="10">
         <v>0.1907461526587664</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="10">
         <v>-0.50094995939728049</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="9">
         <v>0.90765969716420491</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="9">
         <v>0.79472887519557844</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="9">
         <v>88</v>
       </c>
-      <c r="I9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9">
+      <c r="I9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="9">
         <v>220</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="11">
         <v>0.33533091948693289</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9" s="11">
         <v>-0.50094995939728038</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="9">
         <v>0.88760277652655262</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="9">
         <v>0.99422464569228741</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10">
+      <c r="A10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="9">
         <v>245</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="10">
         <v>0.28563695135255701</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="10">
         <v>0.1900383973849451</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="10">
         <v>-0.54658398328582136</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="9">
         <v>0.91810631103439388</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="9">
         <v>0.81320135496168777</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="9">
         <v>82</v>
       </c>
-      <c r="I10" t="s">
-        <v>13</v>
-      </c>
-      <c r="J10">
+      <c r="I10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="9">
         <v>245</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10" s="11">
         <v>0.30791782199662249</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L10" s="11">
         <v>-0.55066294143110706</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="9">
         <v>0.83516669051833115</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="9">
         <v>0.9361347206604157</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11">
+      <c r="A11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="9">
         <v>255</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="10">
         <v>0.27768378944304928</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="10">
         <v>0.1896693234877895</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="10">
         <v>-0.60565826653338961</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="9">
         <v>0.89301030784777169</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="9">
         <v>0.79318515505394893</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="9">
         <v>88</v>
       </c>
-      <c r="I11" t="s">
-        <v>13</v>
-      </c>
-      <c r="J11">
+      <c r="I11" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" s="9">
         <v>255</v>
       </c>
-      <c r="K11" s="3">
+      <c r="K11" s="11">
         <v>0.29597920621214963</v>
       </c>
-      <c r="L11" s="3">
+      <c r="L11" s="11">
         <v>-0.62842911649134725</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="9">
         <v>0.8108274239858283</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="9">
         <v>0.91193918584431766</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
+      <c r="A12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="9">
         <v>250</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="10">
         <v>0.27944034842554433</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="10">
         <v>0.18833914384614969</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="10">
         <v>-0.60565826653338939</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="9">
         <v>0.89826128088860446</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="9">
         <v>0.79532867041053479</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="9">
         <v>82</v>
       </c>
-      <c r="I12" t="s">
-        <v>13</v>
-      </c>
-      <c r="J12">
+      <c r="I12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="9">
         <v>250</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12" s="11">
         <v>0.30219313649665991</v>
       </c>
-      <c r="L12" s="3">
+      <c r="L12" s="11">
         <v>-0.61060587965594204</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="9">
         <v>0.82214377721375875</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="9">
         <v>0.92316225874150681</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
+      <c r="A13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="9">
         <v>195</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="10">
         <v>0.26825448941494029</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="10">
         <v>0.1859866975107787</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="10">
         <v>-0.50142640432179553</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="9">
         <v>0.8824059383244327</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="9">
         <v>0.77058224493053629</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="9">
         <v>86</v>
       </c>
-      <c r="I13" t="s">
-        <v>13</v>
-      </c>
-      <c r="J13">
+      <c r="I13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J13" s="9">
         <v>195</v>
       </c>
-      <c r="K13" s="3">
+      <c r="K13" s="11">
         <v>0.33822313874911408</v>
       </c>
-      <c r="L13" s="3">
+      <c r="L13" s="11">
         <v>-0.5014264043217953</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="9">
         <v>0.89584878698588399</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="9">
         <v>1.0031475756767181</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14">
+      <c r="A14" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="9">
         <v>15</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="10">
         <v>0.27149450732200497</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="10">
         <v>0.18171773128550811</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="10">
         <v>-0.36212732959695981</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="9">
         <v>0.950315765569819</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="9">
         <v>0.8381281460872525</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="9">
         <v>303</v>
       </c>
-      <c r="I14" t="s">
-        <v>13</v>
-      </c>
-      <c r="J14">
+      <c r="I14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" s="9">
         <v>15</v>
       </c>
-      <c r="K14" s="3">
+      <c r="K14" s="11">
         <v>0.16773552519492421</v>
       </c>
-      <c r="L14" s="3">
+      <c r="L14" s="11">
         <v>-0.60059862787070406</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="9">
         <v>0.60312166792405297</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="9">
         <v>0.63329083980000078</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15">
+      <c r="A15" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="9">
         <v>215</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="10">
         <v>0.26451079098763591</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="10">
         <v>0.1782424091986379</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="10">
         <v>-0.5009499593972806</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="9">
         <v>0.87086578768244838</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="9">
         <v>0.75930548502402129</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="9">
         <v>88</v>
       </c>
-      <c r="I15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J15">
+      <c r="I15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" s="9">
         <v>215</v>
       </c>
-      <c r="K15" s="3">
+      <c r="K15" s="11">
         <v>0.3190319757979021</v>
       </c>
-      <c r="L15" s="3">
+      <c r="L15" s="11">
         <v>-0.50094995939728049</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="9">
         <v>0.85845801696186608</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="9">
         <v>0.95958637139104586</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16">
+      <c r="A16" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="9">
         <v>210</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="10">
         <v>0.26255971657686689</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="10">
         <v>0.17737279590050961</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="10">
         <v>-0.50094995939728049</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="9">
         <v>0.865861172508534</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="9">
         <v>0.75455007827993847</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="9">
         <v>87</v>
       </c>
-      <c r="I16" t="s">
-        <v>13</v>
-      </c>
-      <c r="J16">
+      <c r="I16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" s="9">
         <v>210</v>
       </c>
-      <c r="K16" s="3">
+      <c r="K16" s="11">
         <v>0.33106918006503849</v>
       </c>
-      <c r="L16" s="3">
+      <c r="L16" s="11">
         <v>-0.5009499593972806</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="9">
         <v>0.88057478193007888</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="9">
         <v>0.98741696199068352</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17">
+      <c r="A17" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="9">
         <v>200</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="10">
         <v>0.25566640567563392</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="10">
         <v>0.17470756350995911</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="10">
         <v>-0.5014264043217953</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="9">
         <v>0.84951238066009438</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="9">
         <v>0.73909258910535569</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="9">
         <v>89</v>
       </c>
-      <c r="I17" t="s">
-        <v>13</v>
-      </c>
-      <c r="J17">
+      <c r="I17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17" s="9">
         <v>200</v>
       </c>
-      <c r="K17" s="3">
+      <c r="K17" s="11">
         <v>0.32618707629762289</v>
       </c>
-      <c r="L17" s="3">
+      <c r="L17" s="11">
         <v>-0.50142640432179542</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="9">
         <v>0.87265105956094524</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="9">
         <v>0.97574003884504701</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18">
+      <c r="A18" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="9">
         <v>45</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="10">
         <v>0.24843842385680631</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="10">
         <v>0.17302885610911711</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="10">
         <v>-0.43233171735961379</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="9">
         <v>0.88158486545861992</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="9">
         <v>0.78190310589731093</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="9">
         <v>181</v>
       </c>
-      <c r="I18" t="s">
-        <v>13</v>
-      </c>
-      <c r="J18">
+      <c r="I18" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J18" s="9">
         <v>45</v>
       </c>
-      <c r="K18" s="3">
+      <c r="K18" s="11">
         <v>0.23100529982454041</v>
       </c>
-      <c r="L18" s="3">
+      <c r="L18" s="11">
         <v>-0.49283801881286948</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="9">
         <v>0.74931919698135585</v>
       </c>
-      <c r="N18">
+      <c r="N18" s="9">
         <v>0.8132872471489081</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19">
+      <c r="A19" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="9">
         <v>185</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="10">
         <v>0.24809644593646629</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="10">
         <v>0.17156423954841829</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="10">
         <v>-0.50568996613583517</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="9">
         <v>0.83724522637702581</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="9">
         <v>0.72834428183022637</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="9">
         <v>90</v>
       </c>
-      <c r="I19" t="s">
-        <v>13</v>
-      </c>
-      <c r="J19">
+      <c r="I19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J19" s="9">
         <v>185</v>
       </c>
-      <c r="K19" s="3">
+      <c r="K19" s="11">
         <v>0.31042537258341357</v>
       </c>
-      <c r="L19" s="3">
+      <c r="L19" s="11">
         <v>-0.50568996613583506</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="9">
         <v>0.8489606797235828</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="9">
         <v>0.94729875586645662</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20">
+      <c r="A20" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="9">
         <v>180</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="10">
         <v>0.23892650421896119</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="10">
         <v>0.16701002990308031</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="10">
         <v>-0.50568996613583495</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="9">
         <v>0.81776490849108752</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="9">
         <v>0.71041989762600699</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="9">
         <v>92</v>
       </c>
-      <c r="I20" t="s">
-        <v>13</v>
-      </c>
-      <c r="J20">
+      <c r="I20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J20" s="9">
         <v>180</v>
       </c>
-      <c r="K20" s="3">
+      <c r="K20" s="11">
         <v>0.28482216936501281</v>
       </c>
-      <c r="L20" s="3">
+      <c r="L20" s="11">
         <v>-0.50568996613583517</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="9">
         <v>0.80484717808185757</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="9">
         <v>0.89557744442502574</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21">
+      <c r="A21" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="9">
         <v>190</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="10">
         <v>0.24290255979865849</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="10">
         <v>0.16605681452285229</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="10">
         <v>-0.50142640432179542</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="9">
         <v>0.82437975087224147</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="9">
         <v>0.71692062833966008</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="9">
         <v>92</v>
       </c>
-      <c r="I21" t="s">
-        <v>13</v>
-      </c>
-      <c r="J21">
+      <c r="I21" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J21" s="9">
         <v>190</v>
       </c>
-      <c r="K21" s="3">
+      <c r="K21" s="11">
         <v>0.31082827882667302</v>
       </c>
-      <c r="L21" s="3">
+      <c r="L21" s="11">
         <v>-0.5014264043217953</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="9">
         <v>0.84912729418577226</v>
       </c>
-      <c r="N21">
+      <c r="N21" s="9">
         <v>0.94816071347715969</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22">
+      <c r="A22" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="9">
         <v>35</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="10">
         <v>0.25106769216581992</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="10">
         <v>0.1592197568256408</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="10">
         <v>-0.46339019727816649</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="9">
         <v>0.88656241062210672</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="9">
         <v>0.78790311547275715</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="9">
         <v>203</v>
       </c>
-      <c r="I22" t="s">
-        <v>13</v>
-      </c>
-      <c r="J22">
+      <c r="I22" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J22" s="9">
         <v>35</v>
       </c>
-      <c r="K22" s="3">
+      <c r="K22" s="11">
         <v>0.17801574086648239</v>
       </c>
-      <c r="L22" s="3">
+      <c r="L22" s="11">
         <v>-0.53273782183949603</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="9">
         <v>0.63113691902234148</v>
       </c>
-      <c r="N22">
+      <c r="N22" s="9">
         <v>0.67344261573631314</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23">
+      <c r="A23" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="9">
         <v>205</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="10">
         <v>0.23828622427762849</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="10">
         <v>0.15832029829143621</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="10">
         <v>-0.52030699787591228</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="9">
         <v>0.80678536498936404</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="9">
         <v>0.70279279200945277</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="9">
         <v>92</v>
       </c>
-      <c r="I23" t="s">
-        <v>13</v>
-      </c>
-      <c r="J23">
+      <c r="I23" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J23" s="9">
         <v>205</v>
       </c>
-      <c r="K23" s="3">
+      <c r="K23" s="11">
         <v>0.30591363029163499</v>
       </c>
-      <c r="L23" s="3">
+      <c r="L23" s="11">
         <v>-0.5203069978759125</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="9">
         <v>0.83616272855228235</v>
       </c>
-      <c r="N23">
+      <c r="N23" s="9">
         <v>0.93656122464035374</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24">
+      <c r="A24" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="9">
         <v>75</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="10">
         <v>0.22176410523960929</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="10">
         <v>0.15620413843576439</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="10">
         <v>-0.39609619550174269</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="9">
         <v>0.80317963814518423</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="9">
         <v>0.70901535770511159</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="9">
         <v>153</v>
       </c>
-      <c r="I24" t="s">
-        <v>13</v>
-      </c>
-      <c r="J24">
+      <c r="I24" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J24" s="9">
         <v>75</v>
       </c>
-      <c r="K24" s="3">
+      <c r="K24" s="11">
         <v>0.16459731176954809</v>
       </c>
-      <c r="L24" s="3">
+      <c r="L24" s="11">
         <v>-0.54261299907744509</v>
       </c>
-      <c r="M24">
+      <c r="M24" s="9">
         <v>0.59200146937961418</v>
       </c>
-      <c r="N24">
+      <c r="N24" s="9">
         <v>0.62917217380130663</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25">
+      <c r="A25" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="9">
         <v>150</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="10">
         <v>0.21503768734764961</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="10">
         <v>0.1552963477529834</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="10">
         <v>-0.43805991111175152</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="9">
         <v>0.7670195623064705</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="9">
         <v>0.67384219885142538</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="9">
         <v>120</v>
       </c>
-      <c r="I25" t="s">
-        <v>13</v>
-      </c>
-      <c r="J25">
+      <c r="I25" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J25" s="9">
         <v>150</v>
       </c>
-      <c r="K25" s="3">
+      <c r="K25" s="11">
         <v>0.2282638813206512</v>
       </c>
-      <c r="L25" s="3">
+      <c r="L25" s="11">
         <v>-0.52865512921451718</v>
       </c>
-      <c r="M25">
+      <c r="M25" s="9">
         <v>0.70395031706562827</v>
       </c>
-      <c r="N25">
+      <c r="N25" s="9">
         <v>0.78521260795825953</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B26">
+      <c r="A26" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="9">
         <v>175</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="10">
         <v>0.2211507961162609</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="10">
         <v>0.15071562346880829</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="10">
         <v>-0.50568996613583517</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="9">
         <v>0.7745514501305808</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="9">
         <v>0.67113802019037039</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="9">
         <v>94</v>
       </c>
-      <c r="I26" t="s">
-        <v>13</v>
-      </c>
-      <c r="J26">
+      <c r="I26" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J26" s="9">
         <v>175</v>
       </c>
-      <c r="K26" s="3">
+      <c r="K26" s="11">
         <v>0.26632359206274181</v>
       </c>
-      <c r="L26" s="3">
+      <c r="L26" s="11">
         <v>-0.50568996613583495</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="9">
         <v>0.77116068068604104</v>
       </c>
-      <c r="N26">
+      <c r="N26" s="9">
         <v>0.85648910261381184</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27">
+      <c r="A27" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="9">
         <v>165</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="10">
         <v>0.2194483327113306</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="10">
         <v>0.1504835465102439</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="10">
         <v>-0.50568996613583517</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="9">
         <v>0.77082147484083929</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="9">
         <v>0.67063040447478994</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="9">
         <v>104</v>
       </c>
-      <c r="I27" t="s">
-        <v>13</v>
-      </c>
-      <c r="J27">
+      <c r="I27" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J27" s="9">
         <v>165</v>
       </c>
-      <c r="K27" s="3">
+      <c r="K27" s="11">
         <v>0.2353500043515464</v>
       </c>
-      <c r="L27" s="3">
+      <c r="L27" s="11">
         <v>-0.50568996613583517</v>
       </c>
-      <c r="M27">
+      <c r="M27" s="9">
         <v>0.71466234256621131</v>
       </c>
-      <c r="N27">
+      <c r="N27" s="9">
         <v>0.79188499078947716</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28">
+      <c r="A28" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="9">
         <v>50</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="10">
         <v>0.21728566532882129</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="10">
         <v>0.14915507762981831</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="10">
         <v>-0.44978975762618778</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="9">
         <v>0.7989337047732582</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="9">
         <v>0.70384925866406167</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="9">
         <v>183</v>
       </c>
-      <c r="I28" t="s">
-        <v>13</v>
-      </c>
-      <c r="J28">
+      <c r="I28" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J28" s="9">
         <v>50</v>
       </c>
-      <c r="K28" s="3">
+      <c r="K28" s="11">
         <v>0.18327953791507781</v>
       </c>
-      <c r="L28" s="3">
+      <c r="L28" s="11">
         <v>-0.57640128378712119</v>
       </c>
-      <c r="M28">
+      <c r="M28" s="9">
         <v>0.63930137310934021</v>
       </c>
-      <c r="N28">
+      <c r="N28" s="9">
         <v>0.68726234294402366</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29">
+      <c r="A29" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="9">
         <v>40</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="10">
         <v>0.22785147499790989</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="10">
         <v>0.1486700058549548</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="10">
         <v>-0.43233171735961379</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="9">
         <v>0.82426196183527656</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="9">
         <v>0.7324043352366415</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="9">
         <v>193</v>
       </c>
-      <c r="I29" t="s">
-        <v>13</v>
-      </c>
-      <c r="J29">
+      <c r="I29" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J29" s="9">
         <v>40</v>
       </c>
-      <c r="K29" s="3">
+      <c r="K29" s="11">
         <v>0.1679130615251303</v>
       </c>
-      <c r="L29" s="3">
+      <c r="L29" s="11">
         <v>-0.54543460498063667</v>
       </c>
-      <c r="M29">
+      <c r="M29" s="9">
         <v>0.6061676264628304</v>
       </c>
-      <c r="N29">
+      <c r="N29" s="9">
         <v>0.6490052749173284</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30">
+      <c r="A30" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="9">
         <v>170</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="10">
         <v>0.2126524979476199</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="10">
         <v>0.14212548996323121</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="10">
         <v>-0.50568996613583517</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="9">
         <v>0.7547755790623133</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="9">
         <v>0.65545653574116491</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="9">
         <v>100</v>
       </c>
-      <c r="I30" t="s">
-        <v>13</v>
-      </c>
-      <c r="J30">
+      <c r="I30" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J30" s="9">
         <v>170</v>
       </c>
-      <c r="K30" s="3">
+      <c r="K30" s="11">
         <v>0.24761975011633511</v>
       </c>
-      <c r="L30" s="3">
+      <c r="L30" s="11">
         <v>-0.50568996613583517</v>
       </c>
-      <c r="M30">
+      <c r="M30" s="9">
         <v>0.7373498288327438</v>
       </c>
-      <c r="N30">
+      <c r="N30" s="9">
         <v>0.81888292333728463</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>12</v>
-      </c>
-      <c r="B31">
+      <c r="A31" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="9">
         <v>160</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="10">
         <v>0.20563065634649649</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="10">
         <v>0.141843782877106</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="10">
         <v>-0.51408817964922149</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="9">
         <v>0.73493368691887728</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="9">
         <v>0.63504766183941597</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="9">
         <v>108</v>
       </c>
-      <c r="I31" t="s">
-        <v>13</v>
-      </c>
-      <c r="J31">
+      <c r="I31" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J31" s="9">
         <v>160</v>
       </c>
-      <c r="K31" s="3">
+      <c r="K31" s="11">
         <v>0.2213301372249428</v>
       </c>
-      <c r="L31" s="3">
+      <c r="L31" s="11">
         <v>-0.54145270437515247</v>
       </c>
-      <c r="M31">
+      <c r="M31" s="9">
         <v>0.68729585835740281</v>
       </c>
-      <c r="N31">
+      <c r="N31" s="9">
         <v>0.75801949185439887</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32">
+      <c r="A32" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="9">
         <v>145</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32" s="10">
         <v>0.1963858692779297</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="10">
         <v>0.1393726040964143</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="10">
         <v>-0.47050995049425781</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="9">
         <v>0.71995883253547388</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="9">
         <v>0.629661740970619</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="9">
         <v>127</v>
       </c>
-      <c r="I32" t="s">
-        <v>13</v>
-      </c>
-      <c r="J32">
+      <c r="I32" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J32" s="9">
         <v>145</v>
       </c>
-      <c r="K32" s="3">
+      <c r="K32" s="11">
         <v>0.19541171886855091</v>
       </c>
-      <c r="L32" s="3">
+      <c r="L32" s="11">
         <v>-0.58267976388119203</v>
       </c>
-      <c r="M32">
+      <c r="M32" s="9">
         <v>0.64050630616964332</v>
       </c>
-      <c r="N32">
+      <c r="N32" s="9">
         <v>0.70950182637434778</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>12</v>
-      </c>
-      <c r="B33">
+      <c r="A33" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="9">
         <v>60</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C33" s="10">
         <v>0.20243966879492661</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33" s="10">
         <v>0.13879171406563379</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E33" s="10">
         <v>-0.4946762525436551</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="9">
         <v>0.75774685069677827</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="9">
         <v>0.65517859135314005</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="9">
         <v>153</v>
       </c>
-      <c r="I33" t="s">
-        <v>13</v>
-      </c>
-      <c r="J33">
+      <c r="I33" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J33" s="9">
         <v>60</v>
       </c>
-      <c r="K33" s="3">
+      <c r="K33" s="11">
         <v>0.1476925804945475</v>
       </c>
-      <c r="L33" s="3">
+      <c r="L33" s="11">
         <v>-0.63445162976574876</v>
       </c>
-      <c r="M33">
+      <c r="M33" s="9">
         <v>0.55754220306925473</v>
       </c>
-      <c r="N33">
+      <c r="N33" s="9">
         <v>0.58722218963129169</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>12</v>
-      </c>
-      <c r="B34">
+      <c r="A34" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="9">
         <v>80</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" s="10">
         <v>0.20004249730905599</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="10">
         <v>0.13604195950338191</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E34" s="10">
         <v>-0.49912187096670663</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="9">
         <v>0.73996536449629824</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="9">
         <v>0.64520826064627101</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="9">
         <v>148</v>
       </c>
-      <c r="I34" t="s">
-        <v>13</v>
-      </c>
-      <c r="J34">
+      <c r="I34" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J34" s="9">
         <v>80</v>
       </c>
-      <c r="K34" s="3">
+      <c r="K34" s="11">
         <v>0.16250499078424291</v>
       </c>
-      <c r="L34" s="3">
+      <c r="L34" s="11">
         <v>-0.45129805890419122</v>
       </c>
-      <c r="M34">
+      <c r="M34" s="9">
         <v>0.58441005056903772</v>
       </c>
-      <c r="N34">
+      <c r="N34" s="9">
         <v>0.61894476366774331</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>12</v>
-      </c>
-      <c r="B35">
+      <c r="A35" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="9">
         <v>70</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C35" s="10">
         <v>0.19870156470539421</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="10">
         <v>0.13496007485160399</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="10">
         <v>-0.44836250870075661</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="9">
         <v>0.74252411238231431</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="9">
         <v>0.64745610884039939</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="9">
         <v>151</v>
       </c>
-      <c r="I35" t="s">
-        <v>13</v>
-      </c>
-      <c r="J35">
+      <c r="I35" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J35" s="9">
         <v>70</v>
       </c>
-      <c r="K35" s="3">
+      <c r="K35" s="11">
         <v>0.12972234623927029</v>
       </c>
-      <c r="L35" s="3">
+      <c r="L35" s="11">
         <v>-0.62639922444766249</v>
       </c>
-      <c r="M35">
+      <c r="M35" s="9">
         <v>0.5131652130196237</v>
       </c>
-      <c r="N35">
+      <c r="N35" s="9">
         <v>0.54017864835879137</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>12</v>
-      </c>
-      <c r="B36">
+      <c r="A36" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="9">
         <v>155</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C36" s="10">
         <v>0.19336628461512409</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36" s="10">
         <v>0.13272672619494849</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E36" s="10">
         <v>-0.52591673135903305</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="9">
         <v>0.70501305716616058</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="9">
         <v>0.60623711229591237</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="9">
         <v>120</v>
       </c>
-      <c r="I36" t="s">
-        <v>13</v>
-      </c>
-      <c r="J36">
+      <c r="I36" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J36" s="9">
         <v>155</v>
       </c>
-      <c r="K36" s="3">
+      <c r="K36" s="11">
         <v>0.2013370397890355</v>
       </c>
-      <c r="L36" s="3">
+      <c r="L36" s="11">
         <v>-0.52761028231920604</v>
       </c>
-      <c r="M36">
+      <c r="M36" s="9">
         <v>0.64882994858675225</v>
       </c>
-      <c r="N36">
+      <c r="N36" s="9">
         <v>0.71301487046346457</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>12</v>
-      </c>
-      <c r="B37">
+      <c r="A37" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="9">
         <v>55</v>
       </c>
-      <c r="C37" s="6">
+      <c r="C37" s="10">
         <v>0.19681930658199631</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D37" s="10">
         <v>0.12801635215785279</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E37" s="10">
         <v>-0.48954778610862731</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="9">
         <v>0.73902541369125274</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="9">
         <v>0.63909282966886971</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="9">
         <v>167</v>
       </c>
-      <c r="I37" t="s">
-        <v>13</v>
-      </c>
-      <c r="J37">
+      <c r="I37" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J37" s="9">
         <v>55</v>
       </c>
-      <c r="K37" s="3">
+      <c r="K37" s="11">
         <v>0.12588938462982011</v>
       </c>
-      <c r="L37" s="3">
+      <c r="L37" s="11">
         <v>-0.69260971433997387</v>
       </c>
-      <c r="M37">
+      <c r="M37" s="9">
         <v>0.50613401655734036</v>
       </c>
-      <c r="N37">
+      <c r="N37" s="9">
         <v>0.53517685911489188</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>12</v>
-      </c>
-      <c r="B38">
+      <c r="A38" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="9">
         <v>85</v>
       </c>
-      <c r="C38" s="6">
+      <c r="C38" s="10">
         <v>0.19413077393329939</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D38" s="10">
         <v>0.12751520871130159</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E38" s="10">
         <v>-0.47137713306832002</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="9">
         <v>0.72474660982049011</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="9">
         <v>0.63007391737389173</v>
       </c>
-      <c r="H38">
+      <c r="H38" s="9">
         <v>146</v>
       </c>
-      <c r="I38" t="s">
-        <v>13</v>
-      </c>
-      <c r="J38">
+      <c r="I38" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J38" s="9">
         <v>85</v>
       </c>
-      <c r="K38" s="3">
+      <c r="K38" s="11">
         <v>0.1643480719852477</v>
       </c>
-      <c r="L38" s="3">
+      <c r="L38" s="11">
         <v>-0.49099664762346318</v>
       </c>
-      <c r="M38">
+      <c r="M38" s="9">
         <v>0.5878887351790465</v>
       </c>
-      <c r="N38">
+      <c r="N38" s="9">
         <v>0.62206061013400515</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>12</v>
-      </c>
-      <c r="B39">
+      <c r="A39" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="9">
         <v>65</v>
       </c>
-      <c r="C39" s="6">
+      <c r="C39" s="10">
         <v>0.18881116769104159</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D39" s="10">
         <v>0.12633088656138189</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E39" s="10">
         <v>-0.49678243846765741</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="9">
         <v>0.71677607979746671</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="9">
         <v>0.61661284682090001</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="9">
         <v>143</v>
       </c>
-      <c r="I39" t="s">
-        <v>13</v>
-      </c>
-      <c r="J39">
+      <c r="I39" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J39" s="9">
         <v>65</v>
       </c>
-      <c r="K39" s="3">
+      <c r="K39" s="11">
         <v>0.1073636364732007</v>
       </c>
-      <c r="L39" s="3">
+      <c r="L39" s="11">
         <v>-0.69350624419750395</v>
       </c>
-      <c r="M39">
+      <c r="M39" s="9">
         <v>0.46141534320931571</v>
       </c>
-      <c r="N39">
+      <c r="N39" s="9">
         <v>0.48158732577071239</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>12</v>
-      </c>
-      <c r="B40">
+      <c r="A40" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="9">
         <v>140</v>
       </c>
-      <c r="C40" s="6">
+      <c r="C40" s="10">
         <v>0.17164531347829801</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D40" s="10">
         <v>0.11623077239408031</v>
       </c>
-      <c r="E40" s="6">
+      <c r="E40" s="10">
         <v>-0.52804355872903541</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="9">
         <v>0.65764676969898017</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="9">
         <v>0.56932449457409939</v>
       </c>
-      <c r="H40">
+      <c r="H40" s="9">
         <v>129</v>
       </c>
-      <c r="I40" t="s">
-        <v>13</v>
-      </c>
-      <c r="J40">
+      <c r="I40" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J40" s="9">
         <v>140</v>
       </c>
-      <c r="K40" s="3">
+      <c r="K40" s="11">
         <v>0.16065986746198441</v>
       </c>
-      <c r="L40" s="3">
+      <c r="L40" s="11">
         <v>-0.60690804963985423</v>
       </c>
-      <c r="M40">
+      <c r="M40" s="9">
         <v>0.57070541904547378</v>
       </c>
-      <c r="N40">
+      <c r="N40" s="9">
         <v>0.62669254943593455</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>12</v>
-      </c>
-      <c r="B41">
+      <c r="A41" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" s="9">
         <v>135</v>
       </c>
-      <c r="C41" s="6">
+      <c r="C41" s="10">
         <v>0.16739777109131279</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D41" s="10">
         <v>0.1114507595400622</v>
       </c>
-      <c r="E41" s="6">
+      <c r="E41" s="10">
         <v>-0.53943387491566153</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="9">
         <v>0.64657171755455289</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="9">
         <v>0.55934419467522301</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="9">
         <v>136</v>
       </c>
-      <c r="I41" t="s">
-        <v>13</v>
-      </c>
-      <c r="J41">
+      <c r="I41" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J41" s="9">
         <v>135</v>
       </c>
-      <c r="K41" s="3">
+      <c r="K41" s="11">
         <v>0.1588277970333363</v>
       </c>
-      <c r="L41" s="3">
+      <c r="L41" s="11">
         <v>-0.58369265629082812</v>
       </c>
-      <c r="M41">
+      <c r="M41" s="9">
         <v>0.56753246610272068</v>
       </c>
-      <c r="N41">
+      <c r="N41" s="9">
         <v>0.62170708848956258</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>12</v>
-      </c>
-      <c r="B42">
+      <c r="A42" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="9">
         <v>105</v>
       </c>
-      <c r="C42" s="6">
+      <c r="C42" s="10">
         <v>0.17421649621304841</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D42" s="10">
         <v>0.1039702335301287</v>
       </c>
-      <c r="E42" s="6">
+      <c r="E42" s="10">
         <v>-0.63158970790969104</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="9">
         <v>0.67221113971178925</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="9">
         <v>0.57541970933414799</v>
       </c>
-      <c r="H42">
+      <c r="H42" s="9">
         <v>125</v>
       </c>
-      <c r="I42" t="s">
-        <v>13</v>
-      </c>
-      <c r="J42">
+      <c r="I42" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J42" s="9">
         <v>105</v>
       </c>
-      <c r="K42" s="3">
+      <c r="K42" s="11">
         <v>0.1137211325077512</v>
       </c>
-      <c r="L42" s="3">
+      <c r="L42" s="11">
         <v>-0.59913604369105633</v>
       </c>
-      <c r="M42">
+      <c r="M42" s="9">
         <v>0.47293089691084311</v>
       </c>
-      <c r="N42">
+      <c r="N42" s="9">
         <v>0.50701735869274078</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>12</v>
-      </c>
-      <c r="B43">
+      <c r="A43" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" s="9">
         <v>125</v>
       </c>
-      <c r="C43" s="6">
+      <c r="C43" s="10">
         <v>0.1613377791353168</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D43" s="10">
         <v>0.1011705613249352</v>
       </c>
-      <c r="E43" s="6">
+      <c r="E43" s="10">
         <v>-0.61935232541004626</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="9">
         <v>0.63494271847441164</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="9">
         <v>0.54256987318634442</v>
       </c>
-      <c r="H43">
+      <c r="H43" s="9">
         <v>128</v>
       </c>
-      <c r="I43" t="s">
-        <v>13</v>
-      </c>
-      <c r="J43">
+      <c r="I43" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J43" s="9">
         <v>125</v>
       </c>
-      <c r="K43" s="3">
+      <c r="K43" s="11">
         <v>0.13506169640822319</v>
       </c>
-      <c r="L43" s="3">
+      <c r="L43" s="11">
         <v>-0.54830182536410865</v>
       </c>
-      <c r="M43">
+      <c r="M43" s="9">
         <v>0.5184683946013231</v>
       </c>
-      <c r="N43">
+      <c r="N43" s="9">
         <v>0.56278481952931592</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>12</v>
-      </c>
-      <c r="B44">
+      <c r="A44" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="9">
         <v>110</v>
       </c>
-      <c r="C44" s="6">
+      <c r="C44" s="10">
         <v>0.16441657094188539</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D44" s="10">
         <v>9.7098742131500382E-2</v>
       </c>
-      <c r="E44" s="6">
+      <c r="E44" s="10">
         <v>-0.63685322615493845</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="9">
         <v>0.64426273811435553</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="9">
         <v>0.55245986950001424</v>
       </c>
-      <c r="H44">
+      <c r="H44" s="9">
         <v>131</v>
       </c>
-      <c r="I44" t="s">
-        <v>13</v>
-      </c>
-      <c r="J44">
+      <c r="I44" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J44" s="9">
         <v>110</v>
       </c>
-      <c r="K44" s="3">
+      <c r="K44" s="11">
         <v>0.1220337935394378</v>
       </c>
-      <c r="L44" s="3">
+      <c r="L44" s="11">
         <v>-0.57675047697655646</v>
       </c>
-      <c r="M44">
+      <c r="M44" s="9">
         <v>0.49077438906465432</v>
       </c>
-      <c r="N44">
+      <c r="N44" s="9">
         <v>0.52914195698978916</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>12</v>
-      </c>
-      <c r="B45">
+      <c r="A45" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" s="9">
         <v>100</v>
       </c>
-      <c r="C45" s="6">
+      <c r="C45" s="10">
         <v>0.16416863419996061</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D45" s="10">
         <v>9.6342808150024162E-2</v>
       </c>
-      <c r="E45" s="6">
+      <c r="E45" s="10">
         <v>-0.58404916465801526</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="9">
         <v>0.64274898578850803</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="9">
         <v>0.54720537538981584</v>
       </c>
-      <c r="H45">
+      <c r="H45" s="9">
         <v>133</v>
       </c>
-      <c r="I45" t="s">
-        <v>13</v>
-      </c>
-      <c r="J45">
+      <c r="I45" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J45" s="9">
         <v>100</v>
       </c>
-      <c r="K45" s="3">
+      <c r="K45" s="11">
         <v>0.1056313233099051</v>
       </c>
-      <c r="L45" s="3">
+      <c r="L45" s="11">
         <v>-0.54366198317660519</v>
       </c>
-      <c r="M45">
+      <c r="M45" s="9">
         <v>0.45497199544806199</v>
       </c>
-      <c r="N45">
+      <c r="N45" s="9">
         <v>0.48252120566829881</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>12</v>
-      </c>
-      <c r="B46">
+      <c r="A46" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="9">
         <v>115</v>
       </c>
-      <c r="C46" s="6">
+      <c r="C46" s="10">
         <v>0.1586748432648748</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D46" s="10">
         <v>9.4152924502606483E-2</v>
       </c>
-      <c r="E46" s="6">
+      <c r="E46" s="10">
         <v>-0.60283493719210079</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="9">
         <v>0.62837740029995637</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="9">
         <v>0.53666331637039522</v>
       </c>
-      <c r="H46">
+      <c r="H46" s="9">
         <v>131</v>
       </c>
-      <c r="I46" t="s">
-        <v>13</v>
-      </c>
-      <c r="J46">
+      <c r="I46" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J46" s="9">
         <v>115</v>
       </c>
-      <c r="K46" s="3">
+      <c r="K46" s="11">
         <v>0.10571800283326251</v>
       </c>
-      <c r="L46" s="3">
+      <c r="L46" s="11">
         <v>-0.56738766340368096</v>
       </c>
-      <c r="M46">
+      <c r="M46" s="9">
         <v>0.45412552821581581</v>
       </c>
-      <c r="N46">
+      <c r="N46" s="9">
         <v>0.48953497573749882</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>12</v>
-      </c>
-      <c r="B47">
+      <c r="A47" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" s="9">
         <v>5</v>
       </c>
-      <c r="C47" s="6">
+      <c r="C47" s="10">
         <v>0.15371711395369639</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D47" s="10">
         <v>9.4037053219643063E-2</v>
       </c>
-      <c r="E47" s="6">
+      <c r="E47" s="10">
         <v>-0.50248059805520684</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="9">
         <v>0.62604438119915329</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="9">
         <v>0.51718018900153417</v>
       </c>
-      <c r="H47">
+      <c r="H47" s="9">
         <v>561</v>
       </c>
-      <c r="I47" t="s">
-        <v>13</v>
-      </c>
-      <c r="J47">
+      <c r="I47" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J47" s="9">
         <v>5</v>
       </c>
-      <c r="K47" s="3">
+      <c r="K47" s="11">
         <v>5.7164006057994772E-2</v>
       </c>
-      <c r="L47" s="3">
+      <c r="L47" s="11">
         <v>-0.71784594353427855</v>
       </c>
-      <c r="M47">
+      <c r="M47" s="9">
         <v>0.34140979577283909</v>
       </c>
-      <c r="N47">
+      <c r="N47" s="9">
         <v>0.34936457560447037</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>12</v>
-      </c>
-      <c r="B48">
+      <c r="A48" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" s="9">
         <v>95</v>
       </c>
-      <c r="C48" s="6">
+      <c r="C48" s="10">
         <v>0.15940020123797319</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D48" s="10">
         <v>9.3663071614067617E-2</v>
       </c>
-      <c r="E48" s="6">
+      <c r="E48" s="10">
         <v>-0.56887564708758687</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="9">
         <v>0.62968305897094401</v>
       </c>
-      <c r="G48">
+      <c r="G48" s="9">
         <v>0.53755773315318889</v>
       </c>
-      <c r="H48">
+      <c r="H48" s="9">
         <v>142</v>
       </c>
-      <c r="I48" t="s">
-        <v>13</v>
-      </c>
-      <c r="J48">
+      <c r="I48" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J48" s="9">
         <v>95</v>
       </c>
-      <c r="K48" s="3">
+      <c r="K48" s="11">
         <v>0.1133582150825392</v>
       </c>
-      <c r="L48" s="3">
+      <c r="L48" s="11">
         <v>-0.55605488380158818</v>
       </c>
-      <c r="M48">
+      <c r="M48" s="9">
         <v>0.47264560742582518</v>
       </c>
-      <c r="N48">
+      <c r="N48" s="9">
         <v>0.49939867967214507</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>12</v>
-      </c>
-      <c r="B49">
+      <c r="A49" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="9">
         <v>130</v>
       </c>
-      <c r="C49" s="6">
+      <c r="C49" s="10">
         <v>0.1490122019438225</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D49" s="10">
         <v>9.1998693925014363E-2</v>
       </c>
-      <c r="E49" s="6">
+      <c r="E49" s="10">
         <v>-0.62923164974709267</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="9">
         <v>0.60065084284786097</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="9">
         <v>0.51311922850437819</v>
       </c>
-      <c r="H49">
+      <c r="H49" s="9">
         <v>131</v>
       </c>
-      <c r="I49" t="s">
-        <v>13</v>
-      </c>
-      <c r="J49">
+      <c r="I49" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J49" s="9">
         <v>130</v>
       </c>
-      <c r="K49" s="3">
+      <c r="K49" s="11">
         <v>0.13068592043343499</v>
       </c>
-      <c r="L49" s="3">
+      <c r="L49" s="11">
         <v>-0.56013604354090729</v>
       </c>
-      <c r="M49">
+      <c r="M49" s="9">
         <v>0.50871270666408086</v>
       </c>
-      <c r="N49">
+      <c r="N49" s="9">
         <v>0.55285453793543238</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>12</v>
-      </c>
-      <c r="B50">
+      <c r="A50" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B50" s="9">
         <v>90</v>
       </c>
-      <c r="C50" s="6">
+      <c r="C50" s="10">
         <v>0.15870713949299381</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D50" s="10">
         <v>9.1160190614004932E-2</v>
       </c>
-      <c r="E50" s="6">
+      <c r="E50" s="10">
         <v>-0.4859824048776612</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="9">
         <v>0.62785936429070011</v>
       </c>
-      <c r="G50">
+      <c r="G50" s="9">
         <v>0.54128371438961687</v>
       </c>
-      <c r="H50">
+      <c r="H50" s="9">
         <v>154</v>
       </c>
-      <c r="I50" t="s">
-        <v>13</v>
-      </c>
-      <c r="J50">
+      <c r="I50" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J50" s="9">
         <v>90</v>
       </c>
-      <c r="K50" s="3">
+      <c r="K50" s="11">
         <v>0.12770362186077541</v>
       </c>
-      <c r="L50" s="3">
+      <c r="L50" s="11">
         <v>-0.54413616919594432</v>
       </c>
-      <c r="M50">
+      <c r="M50" s="9">
         <v>0.5054099799134012</v>
       </c>
-      <c r="N50">
+      <c r="N50" s="9">
         <v>0.5355912146025138</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>12</v>
-      </c>
-      <c r="B51">
+      <c r="A51" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" s="9">
         <v>10</v>
       </c>
-      <c r="C51" s="6">
+      <c r="C51" s="10">
         <v>0.14958777958505201</v>
       </c>
-      <c r="D51" s="6">
+      <c r="D51" s="10">
         <v>9.0085486818736404E-2</v>
       </c>
-      <c r="E51" s="6">
+      <c r="E51" s="10">
         <v>-0.50754724745100721</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="9">
         <v>0.61626321941012618</v>
       </c>
-      <c r="G51">
+      <c r="G51" s="9">
         <v>0.51862452793744496</v>
       </c>
-      <c r="H51">
+      <c r="H51" s="9">
         <v>403</v>
       </c>
-      <c r="I51" t="s">
-        <v>13</v>
-      </c>
-      <c r="J51">
+      <c r="I51" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J51" s="9">
         <v>10</v>
       </c>
-      <c r="K51" s="3">
+      <c r="K51" s="11">
         <v>4.6573674256561892E-2</v>
       </c>
-      <c r="L51" s="3">
+      <c r="L51" s="11">
         <v>-0.70374257705833021</v>
       </c>
-      <c r="M51">
+      <c r="M51" s="9">
         <v>0.31275751281563391</v>
       </c>
-      <c r="N51">
+      <c r="N51" s="9">
         <v>0.31890767658861091</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>12</v>
-      </c>
-      <c r="B52">
+      <c r="A52" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="9">
         <v>120</v>
       </c>
-      <c r="C52" s="6">
+      <c r="C52" s="10">
         <v>0.14752244188661481</v>
       </c>
-      <c r="D52" s="6">
+      <c r="D52" s="10">
         <v>8.1302005373330433E-2</v>
       </c>
-      <c r="E52" s="6">
+      <c r="E52" s="10">
         <v>-0.58626076661528259</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="9">
         <v>0.59638365588137277</v>
       </c>
-      <c r="G52">
+      <c r="G52" s="9">
         <v>0.50908578624097711</v>
       </c>
-      <c r="H52">
+      <c r="H52" s="9">
         <v>136</v>
       </c>
-      <c r="I52" t="s">
-        <v>13</v>
-      </c>
-      <c r="J52">
+      <c r="I52" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J52" s="9">
         <v>120</v>
       </c>
-      <c r="K52" s="3">
+      <c r="K52" s="11">
         <v>0.1181624599597639</v>
       </c>
-      <c r="L52" s="3">
+      <c r="L52" s="11">
         <v>-0.56033103673743634</v>
       </c>
-      <c r="M52">
+      <c r="M52" s="9">
         <v>0.48159739565221049</v>
       </c>
-      <c r="N52">
+      <c r="N52" s="9">
         <v>0.52011107983376137</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2783,10 +2807,13 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -2809,10 +2836,10 @@
       <c r="A2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="4">
         <v>0.36389744661854012</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="4">
         <v>-0.81659847022030041</v>
       </c>
       <c r="D2">

</xml_diff>